<commit_message>
fix number of nodes
</commit_message>
<xml_diff>
--- a/classifier/data/classifier_result/classifier_results.xlsx
+++ b/classifier/data/classifier_result/classifier_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="37">
   <si>
     <t>Correlation threshold</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>power_graph= 2,add_neighbors_from_adj_matrix,rw_on_main_graph</t>
+  </si>
+  <si>
+    <t>power_graph= 2,</t>
+  </si>
+  <si>
+    <t>power_graph= 2,weigted_randomwalk</t>
+  </si>
+  <si>
+    <t>power_graph= 2,rw_on_main_graph</t>
   </si>
   <si>
     <t>{'vector_size': 10, 'window_size': 5, 'learning_rate': 0.001, 'min_learning_rate': 0.0001, 'min_count': 1, 'min_vocab_size': 'None', 'workers': 4, 'epochs': 50}</t>
@@ -473,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="Z2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -716,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="Z3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -796,7 +805,7 @@
         <v>10</v>
       </c>
       <c r="Z4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -876,7 +885,7 @@
         <v>10</v>
       </c>
       <c r="Z5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -956,7 +965,7 @@
         <v>10</v>
       </c>
       <c r="Z6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1036,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="Z7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1116,7 +1125,7 @@
         <v>10</v>
       </c>
       <c r="Z8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1196,7 +1205,7 @@
         <v>10</v>
       </c>
       <c r="Z9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1276,7 +1285,1767 @@
         <v>10</v>
       </c>
       <c r="Z10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>0.8169510638297872</v>
+      </c>
+      <c r="H11">
+        <v>0.7616442852446496</v>
+      </c>
+      <c r="I11">
+        <v>0.8056069582397545</v>
+      </c>
+      <c r="J11">
+        <v>0.7233716119417347</v>
+      </c>
+      <c r="K11">
+        <v>26.7</v>
+      </c>
+      <c r="L11">
+        <v>42</v>
+      </c>
+      <c r="M11">
+        <v>110.1</v>
+      </c>
+      <c r="N11">
+        <v>196.5</v>
+      </c>
+      <c r="O11">
+        <v>0.7365272938443669</v>
+      </c>
+      <c r="P11">
+        <v>0.6378433896080955</v>
+      </c>
+      <c r="Q11">
+        <v>0.6978715973568914</v>
+      </c>
+      <c r="R11">
+        <v>0.5975395811618722</v>
+      </c>
+      <c r="S11">
+        <v>42</v>
+      </c>
+      <c r="T11">
+        <v>68</v>
+      </c>
+      <c r="U11">
+        <v>101</v>
+      </c>
+      <c r="V11">
+        <v>206</v>
+      </c>
+      <c r="W11">
+        <v>3753</v>
+      </c>
+      <c r="X11">
+        <v>417</v>
+      </c>
+      <c r="Y11">
+        <v>10</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12">
+        <v>0.7</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>0.8052255319148935</v>
+      </c>
+      <c r="H12">
+        <v>0.7405244217198456</v>
+      </c>
+      <c r="I12">
+        <v>0.8028623331632154</v>
+      </c>
+      <c r="J12">
+        <v>0.6904084637167344</v>
+      </c>
+      <c r="K12">
+        <v>26.1</v>
+      </c>
+      <c r="L12">
+        <v>47</v>
+      </c>
+      <c r="M12">
+        <v>105.1</v>
+      </c>
+      <c r="N12">
+        <v>197.1</v>
+      </c>
+      <c r="O12">
+        <v>0.6977351916376305</v>
+      </c>
+      <c r="P12">
+        <v>0.5921606201620433</v>
+      </c>
+      <c r="Q12">
+        <v>0.6635503711974301</v>
+      </c>
+      <c r="R12">
+        <v>0.5513972302207596</v>
+      </c>
+      <c r="S12">
+        <v>49</v>
+      </c>
+      <c r="T12">
+        <v>77</v>
+      </c>
+      <c r="U12">
+        <v>92</v>
+      </c>
+      <c r="V12">
+        <v>199</v>
+      </c>
+      <c r="W12">
+        <v>3753</v>
+      </c>
+      <c r="X12">
+        <v>417</v>
+      </c>
+      <c r="Y12">
+        <v>10</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13">
+        <v>0.7</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
         <v>33</v>
+      </c>
+      <c r="G13">
+        <v>0.746068085106383</v>
+      </c>
+      <c r="H13">
+        <v>0.5752151954820457</v>
+      </c>
+      <c r="I13">
+        <v>0.8919296142556103</v>
+      </c>
+      <c r="J13">
+        <v>0.4250185099451113</v>
+      </c>
+      <c r="K13">
+        <v>7.9</v>
+      </c>
+      <c r="L13">
+        <v>87.40000000000001</v>
+      </c>
+      <c r="M13">
+        <v>64.7</v>
+      </c>
+      <c r="N13">
+        <v>215.3</v>
+      </c>
+      <c r="O13">
+        <v>0.6908246225319395</v>
+      </c>
+      <c r="P13">
+        <v>0.4529432108699843</v>
+      </c>
+      <c r="Q13">
+        <v>0.821547619047619</v>
+      </c>
+      <c r="R13">
+        <v>0.3224724802201583</v>
+      </c>
+      <c r="S13">
+        <v>12</v>
+      </c>
+      <c r="T13">
+        <v>117</v>
+      </c>
+      <c r="U13">
+        <v>52</v>
+      </c>
+      <c r="V13">
+        <v>236</v>
+      </c>
+      <c r="W13">
+        <v>3753</v>
+      </c>
+      <c r="X13">
+        <v>417</v>
+      </c>
+      <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14">
+        <v>0.7</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14">
+        <v>0.8089574468085108</v>
+      </c>
+      <c r="H14">
+        <v>0.7486569660748663</v>
+      </c>
+      <c r="I14">
+        <v>0.8018333769230669</v>
+      </c>
+      <c r="J14">
+        <v>0.7031568087169737</v>
+      </c>
+      <c r="K14">
+        <v>26.6</v>
+      </c>
+      <c r="L14">
+        <v>45.1</v>
+      </c>
+      <c r="M14">
+        <v>107</v>
+      </c>
+      <c r="N14">
+        <v>196.6</v>
+      </c>
+      <c r="O14">
+        <v>0.7242160278745644</v>
+      </c>
+      <c r="P14">
+        <v>0.6181811742618194</v>
+      </c>
+      <c r="Q14">
+        <v>0.6936270965876228</v>
+      </c>
+      <c r="R14">
+        <v>0.564942645074224</v>
+      </c>
+      <c r="S14">
+        <v>42</v>
+      </c>
+      <c r="T14">
+        <v>73</v>
+      </c>
+      <c r="U14">
+        <v>96</v>
+      </c>
+      <c r="V14">
+        <v>206</v>
+      </c>
+      <c r="W14">
+        <v>3753</v>
+      </c>
+      <c r="X14">
+        <v>417</v>
+      </c>
+      <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15">
+        <v>0.7</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>0.8092283687943264</v>
+      </c>
+      <c r="H15">
+        <v>0.7495139087580067</v>
+      </c>
+      <c r="I15">
+        <v>0.8013985992541752</v>
+      </c>
+      <c r="J15">
+        <v>0.7050274765140123</v>
+      </c>
+      <c r="K15">
+        <v>26.8</v>
+      </c>
+      <c r="L15">
+        <v>44.8</v>
+      </c>
+      <c r="M15">
+        <v>107.3</v>
+      </c>
+      <c r="N15">
+        <v>196.4</v>
+      </c>
+      <c r="O15">
+        <v>0.7172473867595818</v>
+      </c>
+      <c r="P15">
+        <v>0.6062790378696907</v>
+      </c>
+      <c r="Q15">
+        <v>0.6955104617604617</v>
+      </c>
+      <c r="R15">
+        <v>0.5623909131803869</v>
+      </c>
+      <c r="S15">
+        <v>43</v>
+      </c>
+      <c r="T15">
+        <v>75</v>
+      </c>
+      <c r="U15">
+        <v>94</v>
+      </c>
+      <c r="V15">
+        <v>205</v>
+      </c>
+      <c r="W15">
+        <v>3753</v>
+      </c>
+      <c r="X15">
+        <v>417</v>
+      </c>
+      <c r="Y15">
+        <v>10</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16">
+        <v>0.7</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16">
+        <v>0.7231595744680851</v>
+      </c>
+      <c r="H16">
+        <v>0.4999100319688555</v>
+      </c>
+      <c r="I16">
+        <v>0.9273284255068619</v>
+      </c>
+      <c r="J16">
+        <v>0.3447098908118581</v>
+      </c>
+      <c r="K16">
+        <v>4.3</v>
+      </c>
+      <c r="L16">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="M16">
+        <v>52.5</v>
+      </c>
+      <c r="N16">
+        <v>218.9</v>
+      </c>
+      <c r="O16">
+        <v>0.6525551684088269</v>
+      </c>
+      <c r="P16">
+        <v>0.3256750585840975</v>
+      </c>
+      <c r="Q16">
+        <v>0.7838095238095237</v>
+      </c>
+      <c r="R16">
+        <v>0.2154578754578755</v>
+      </c>
+      <c r="S16">
+        <v>12</v>
+      </c>
+      <c r="T16">
+        <v>133</v>
+      </c>
+      <c r="U16">
+        <v>36</v>
+      </c>
+      <c r="V16">
+        <v>236</v>
+      </c>
+      <c r="W16">
+        <v>3753</v>
+      </c>
+      <c r="X16">
+        <v>417</v>
+      </c>
+      <c r="Y16">
+        <v>10</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17">
+        <v>0.7</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>0.7972212765957447</v>
+      </c>
+      <c r="H17">
+        <v>0.7209653626219394</v>
+      </c>
+      <c r="I17">
+        <v>0.816876161683853</v>
+      </c>
+      <c r="J17">
+        <v>0.647188502625035</v>
+      </c>
+      <c r="K17">
+        <v>22.5</v>
+      </c>
+      <c r="L17">
+        <v>53.6</v>
+      </c>
+      <c r="M17">
+        <v>98.5</v>
+      </c>
+      <c r="N17">
+        <v>200.7</v>
+      </c>
+      <c r="O17">
+        <v>0.7216608594657374</v>
+      </c>
+      <c r="P17">
+        <v>0.6157244206449206</v>
+      </c>
+      <c r="Q17">
+        <v>0.7287325174825176</v>
+      </c>
+      <c r="R17">
+        <v>0.5519294559929235</v>
+      </c>
+      <c r="S17">
+        <v>40</v>
+      </c>
+      <c r="T17">
+        <v>76</v>
+      </c>
+      <c r="U17">
+        <v>93</v>
+      </c>
+      <c r="V17">
+        <v>208</v>
+      </c>
+      <c r="W17">
+        <v>3753</v>
+      </c>
+      <c r="X17">
+        <v>417</v>
+      </c>
+      <c r="Y17">
+        <v>10</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18">
+        <v>0.7</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18">
+        <v>0.7929709219858158</v>
+      </c>
+      <c r="H18">
+        <v>0.6992118588263764</v>
+      </c>
+      <c r="I18">
+        <v>0.8471432282629626</v>
+      </c>
+      <c r="J18">
+        <v>0.5977166610365653</v>
+      </c>
+      <c r="K18">
+        <v>16.7</v>
+      </c>
+      <c r="L18">
+        <v>61</v>
+      </c>
+      <c r="M18">
+        <v>91.09999999999999</v>
+      </c>
+      <c r="N18">
+        <v>206.5</v>
+      </c>
+      <c r="O18">
+        <v>0.6952380952380951</v>
+      </c>
+      <c r="P18">
+        <v>0.5498919717901851</v>
+      </c>
+      <c r="Q18">
+        <v>0.6960678210678212</v>
+      </c>
+      <c r="R18">
+        <v>0.4679438827426444</v>
+      </c>
+      <c r="S18">
+        <v>34</v>
+      </c>
+      <c r="T18">
+        <v>93</v>
+      </c>
+      <c r="U18">
+        <v>76</v>
+      </c>
+      <c r="V18">
+        <v>214</v>
+      </c>
+      <c r="W18">
+        <v>3753</v>
+      </c>
+      <c r="X18">
+        <v>417</v>
+      </c>
+      <c r="Y18">
+        <v>10</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19">
+        <v>0.7</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19">
+        <v>0.7295517730496454</v>
+      </c>
+      <c r="H19">
+        <v>0.5322098099250741</v>
+      </c>
+      <c r="I19">
+        <v>0.8805688769591056</v>
+      </c>
+      <c r="J19">
+        <v>0.3846487097835496</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>93.5</v>
+      </c>
+      <c r="M19">
+        <v>58.6</v>
+      </c>
+      <c r="N19">
+        <v>215.2</v>
+      </c>
+      <c r="O19">
+        <v>0.6477932636469221</v>
+      </c>
+      <c r="P19">
+        <v>0.3530618866916507</v>
+      </c>
+      <c r="Q19">
+        <v>0.7036507936507936</v>
+      </c>
+      <c r="R19">
+        <v>0.2447263928881576</v>
+      </c>
+      <c r="S19">
+        <v>19</v>
+      </c>
+      <c r="T19">
+        <v>128</v>
+      </c>
+      <c r="U19">
+        <v>41</v>
+      </c>
+      <c r="V19">
+        <v>229</v>
+      </c>
+      <c r="W19">
+        <v>3753</v>
+      </c>
+      <c r="X19">
+        <v>417</v>
+      </c>
+      <c r="Y19">
+        <v>10</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20">
+        <v>-0.7</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>0.8366609929078015</v>
+      </c>
+      <c r="H20">
+        <v>0.7791527621724487</v>
+      </c>
+      <c r="I20">
+        <v>0.8617974416576253</v>
+      </c>
+      <c r="J20">
+        <v>0.7114518345752874</v>
+      </c>
+      <c r="K20">
+        <v>17.4</v>
+      </c>
+      <c r="L20">
+        <v>43.9</v>
+      </c>
+      <c r="M20">
+        <v>108.2</v>
+      </c>
+      <c r="N20">
+        <v>205.8</v>
+      </c>
+      <c r="O20">
+        <v>0.7670150987224157</v>
+      </c>
+      <c r="P20">
+        <v>0.6592834383204239</v>
+      </c>
+      <c r="Q20">
+        <v>0.8107897004955827</v>
+      </c>
+      <c r="R20">
+        <v>0.5802272838960144</v>
+      </c>
+      <c r="S20">
+        <v>24</v>
+      </c>
+      <c r="T20">
+        <v>73</v>
+      </c>
+      <c r="U20">
+        <v>96</v>
+      </c>
+      <c r="V20">
+        <v>224</v>
+      </c>
+      <c r="W20">
+        <v>3753</v>
+      </c>
+      <c r="X20">
+        <v>417</v>
+      </c>
+      <c r="Y20">
+        <v>10</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21">
+        <v>-0.7</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>0.8201468085106383</v>
+      </c>
+      <c r="H21">
+        <v>0.7660167481871607</v>
+      </c>
+      <c r="I21">
+        <v>0.8102212116387912</v>
+      </c>
+      <c r="J21">
+        <v>0.7281826943876281</v>
+      </c>
+      <c r="K21">
+        <v>26.2</v>
+      </c>
+      <c r="L21">
+        <v>41.3</v>
+      </c>
+      <c r="M21">
+        <v>110.8</v>
+      </c>
+      <c r="N21">
+        <v>197</v>
+      </c>
+      <c r="O21">
+        <v>0.7264227642276422</v>
+      </c>
+      <c r="P21">
+        <v>0.6124770791127734</v>
+      </c>
+      <c r="Q21">
+        <v>0.7009161761870739</v>
+      </c>
+      <c r="R21">
+        <v>0.5563690476190477</v>
+      </c>
+      <c r="S21">
+        <v>40</v>
+      </c>
+      <c r="T21">
+        <v>74</v>
+      </c>
+      <c r="U21">
+        <v>95</v>
+      </c>
+      <c r="V21">
+        <v>208</v>
+      </c>
+      <c r="W21">
+        <v>3753</v>
+      </c>
+      <c r="X21">
+        <v>417</v>
+      </c>
+      <c r="Y21">
+        <v>10</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22">
+        <v>-0.7</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22">
+        <v>0.7292794326241135</v>
+      </c>
+      <c r="H22">
+        <v>0.5368727908851885</v>
+      </c>
+      <c r="I22">
+        <v>0.8754171272854594</v>
+      </c>
+      <c r="J22">
+        <v>0.3894752566344996</v>
+      </c>
+      <c r="K22">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="L22">
+        <v>92.8</v>
+      </c>
+      <c r="M22">
+        <v>59.3</v>
+      </c>
+      <c r="N22">
+        <v>214.4</v>
+      </c>
+      <c r="O22">
+        <v>0.5828687572590011</v>
+      </c>
+      <c r="P22">
+        <v>0.2832794800291052</v>
+      </c>
+      <c r="Q22">
+        <v>0.4883333333333334</v>
+      </c>
+      <c r="R22">
+        <v>0.2202777777777777</v>
+      </c>
+      <c r="S22">
+        <v>40</v>
+      </c>
+      <c r="T22">
+        <v>134</v>
+      </c>
+      <c r="U22">
+        <v>35</v>
+      </c>
+      <c r="V22">
+        <v>208</v>
+      </c>
+      <c r="W22">
+        <v>3753</v>
+      </c>
+      <c r="X22">
+        <v>417</v>
+      </c>
+      <c r="Y22">
+        <v>10</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23">
+        <v>-0.7</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23">
+        <v>0.8387929078014185</v>
+      </c>
+      <c r="H23">
+        <v>0.7778077399746841</v>
+      </c>
+      <c r="I23">
+        <v>0.8804607310068212</v>
+      </c>
+      <c r="J23">
+        <v>0.6967621329418631</v>
+      </c>
+      <c r="K23">
+        <v>14.4</v>
+      </c>
+      <c r="L23">
+        <v>46.1</v>
+      </c>
+      <c r="M23">
+        <v>106</v>
+      </c>
+      <c r="N23">
+        <v>208.8</v>
+      </c>
+      <c r="O23">
+        <v>0.7293844367015098</v>
+      </c>
+      <c r="P23">
+        <v>0.6156127450980393</v>
+      </c>
+      <c r="Q23">
+        <v>0.7298401598401598</v>
+      </c>
+      <c r="R23">
+        <v>0.5397865704986448</v>
+      </c>
+      <c r="S23">
+        <v>35</v>
+      </c>
+      <c r="T23">
+        <v>78</v>
+      </c>
+      <c r="U23">
+        <v>91</v>
+      </c>
+      <c r="V23">
+        <v>213</v>
+      </c>
+      <c r="W23">
+        <v>3753</v>
+      </c>
+      <c r="X23">
+        <v>417</v>
+      </c>
+      <c r="Y23">
+        <v>10</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24">
+        <v>-0.7</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24">
+        <v>0.8470567375886526</v>
+      </c>
+      <c r="H24">
+        <v>0.7902912772263917</v>
+      </c>
+      <c r="I24">
+        <v>0.889361020393733</v>
+      </c>
+      <c r="J24">
+        <v>0.7113510902694385</v>
+      </c>
+      <c r="K24">
+        <v>13.5</v>
+      </c>
+      <c r="L24">
+        <v>43.9</v>
+      </c>
+      <c r="M24">
+        <v>108.2</v>
+      </c>
+      <c r="N24">
+        <v>209.7</v>
+      </c>
+      <c r="O24">
+        <v>0.7765969802555168</v>
+      </c>
+      <c r="P24">
+        <v>0.680081001928828</v>
+      </c>
+      <c r="Q24">
+        <v>0.8219871794871795</v>
+      </c>
+      <c r="R24">
+        <v>0.5871300186741364</v>
+      </c>
+      <c r="S24">
+        <v>22</v>
+      </c>
+      <c r="T24">
+        <v>71</v>
+      </c>
+      <c r="U24">
+        <v>98</v>
+      </c>
+      <c r="V24">
+        <v>226</v>
+      </c>
+      <c r="W24">
+        <v>3753</v>
+      </c>
+      <c r="X24">
+        <v>417</v>
+      </c>
+      <c r="Y24">
+        <v>10</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25">
+        <v>-0.7</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25">
+        <v>0.7175574468085106</v>
+      </c>
+      <c r="H25">
+        <v>0.490657935842615</v>
+      </c>
+      <c r="I25">
+        <v>0.9113357260677175</v>
+      </c>
+      <c r="J25">
+        <v>0.3364811182343295</v>
+      </c>
+      <c r="K25">
+        <v>5.1</v>
+      </c>
+      <c r="L25">
+        <v>100.9</v>
+      </c>
+      <c r="M25">
+        <v>51.2</v>
+      </c>
+      <c r="N25">
+        <v>218.1</v>
+      </c>
+      <c r="O25">
+        <v>0.5998257839721253</v>
+      </c>
+      <c r="P25">
+        <v>0.2608240760002774</v>
+      </c>
+      <c r="Q25">
+        <v>0.5077380952380952</v>
+      </c>
+      <c r="R25">
+        <v>0.1783439509407002</v>
+      </c>
+      <c r="S25">
+        <v>28</v>
+      </c>
+      <c r="T25">
+        <v>139</v>
+      </c>
+      <c r="U25">
+        <v>30</v>
+      </c>
+      <c r="V25">
+        <v>220</v>
+      </c>
+      <c r="W25">
+        <v>3753</v>
+      </c>
+      <c r="X25">
+        <v>417</v>
+      </c>
+      <c r="Y25">
+        <v>10</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26">
+        <v>-0.7</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26">
+        <v>0.8377255319148936</v>
+      </c>
+      <c r="H26">
+        <v>0.7748895077259673</v>
+      </c>
+      <c r="I26">
+        <v>0.8873712432016909</v>
+      </c>
+      <c r="J26">
+        <v>0.6893547679928747</v>
+      </c>
+      <c r="K26">
+        <v>13.7</v>
+      </c>
+      <c r="L26">
+        <v>47.2</v>
+      </c>
+      <c r="M26">
+        <v>104.9</v>
+      </c>
+      <c r="N26">
+        <v>209.5</v>
+      </c>
+      <c r="O26">
+        <v>0.7361207897793263</v>
+      </c>
+      <c r="P26">
+        <v>0.6113167867527201</v>
+      </c>
+      <c r="Q26">
+        <v>0.7486224886224886</v>
+      </c>
+      <c r="R26">
+        <v>0.5316640866873065</v>
+      </c>
+      <c r="S26">
+        <v>30</v>
+      </c>
+      <c r="T26">
+        <v>80</v>
+      </c>
+      <c r="U26">
+        <v>89</v>
+      </c>
+      <c r="V26">
+        <v>218</v>
+      </c>
+      <c r="W26">
+        <v>3753</v>
+      </c>
+      <c r="X26">
+        <v>417</v>
+      </c>
+      <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27">
+        <v>-0.7</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27">
+        <v>0.8278702127659574</v>
+      </c>
+      <c r="H27">
+        <v>0.7652056427438414</v>
+      </c>
+      <c r="I27">
+        <v>0.853857198476365</v>
+      </c>
+      <c r="J27">
+        <v>0.6942631672603082</v>
+      </c>
+      <c r="K27">
+        <v>18.2</v>
+      </c>
+      <c r="L27">
+        <v>46.4</v>
+      </c>
+      <c r="M27">
+        <v>105.7</v>
+      </c>
+      <c r="N27">
+        <v>205</v>
+      </c>
+      <c r="O27">
+        <v>0.7146922183507549</v>
+      </c>
+      <c r="P27">
+        <v>0.5983679075768858</v>
+      </c>
+      <c r="Q27">
+        <v>0.7003880188439012</v>
+      </c>
+      <c r="R27">
+        <v>0.5493978440831989</v>
+      </c>
+      <c r="S27">
+        <v>41</v>
+      </c>
+      <c r="T27">
+        <v>78</v>
+      </c>
+      <c r="U27">
+        <v>91</v>
+      </c>
+      <c r="V27">
+        <v>207</v>
+      </c>
+      <c r="W27">
+        <v>3753</v>
+      </c>
+      <c r="X27">
+        <v>417</v>
+      </c>
+      <c r="Y27">
+        <v>10</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28">
+        <v>-0.7</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28">
+        <v>0.7431439716312057</v>
+      </c>
+      <c r="H28">
+        <v>0.5506018364820408</v>
+      </c>
+      <c r="I28">
+        <v>0.9406882209753752</v>
+      </c>
+      <c r="J28">
+        <v>0.392298230768762</v>
+      </c>
+      <c r="K28">
+        <v>4.1</v>
+      </c>
+      <c r="L28">
+        <v>92.3</v>
+      </c>
+      <c r="M28">
+        <v>59.8</v>
+      </c>
+      <c r="N28">
+        <v>219.1</v>
+      </c>
+      <c r="O28">
+        <v>0.6333914053426248</v>
+      </c>
+      <c r="P28">
+        <v>0.3558272371750633</v>
+      </c>
+      <c r="Q28">
+        <v>0.6416666666666667</v>
+      </c>
+      <c r="R28">
+        <v>0.2764499484004128</v>
+      </c>
+      <c r="S28">
+        <v>26</v>
+      </c>
+      <c r="T28">
+        <v>127</v>
+      </c>
+      <c r="U28">
+        <v>42</v>
+      </c>
+      <c r="V28">
+        <v>222</v>
+      </c>
+      <c r="W28">
+        <v>3753</v>
+      </c>
+      <c r="X28">
+        <v>417</v>
+      </c>
+      <c r="Y28">
+        <v>10</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29">
+        <v>0.7</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29">
+        <v>0.8036241134751773</v>
+      </c>
+      <c r="H29">
+        <v>0.7214772399168654</v>
+      </c>
+      <c r="I29">
+        <v>0.8477113332116251</v>
+      </c>
+      <c r="J29">
+        <v>0.6283322795775275</v>
+      </c>
+      <c r="K29">
+        <v>17.2</v>
+      </c>
+      <c r="L29">
+        <v>56.5</v>
+      </c>
+      <c r="M29">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="N29">
+        <v>206</v>
+      </c>
+      <c r="O29">
+        <v>0.7552264808362368</v>
+      </c>
+      <c r="P29">
+        <v>0.6324564638611336</v>
+      </c>
+      <c r="Q29">
+        <v>0.7943084693084692</v>
+      </c>
+      <c r="R29">
+        <v>0.5345503464543712</v>
+      </c>
+      <c r="S29">
+        <v>24</v>
+      </c>
+      <c r="T29">
+        <v>78</v>
+      </c>
+      <c r="U29">
+        <v>91</v>
+      </c>
+      <c r="V29">
+        <v>224</v>
+      </c>
+      <c r="W29">
+        <v>3753</v>
+      </c>
+      <c r="X29">
+        <v>417</v>
+      </c>
+      <c r="Y29">
+        <v>10</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30">
+        <v>0.7</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>0.7980276595744681</v>
+      </c>
+      <c r="H30">
+        <v>0.7212953090013718</v>
+      </c>
+      <c r="I30">
+        <v>0.8203742697615988</v>
+      </c>
+      <c r="J30">
+        <v>0.6451911778474336</v>
+      </c>
+      <c r="K30">
+        <v>21.9</v>
+      </c>
+      <c r="L30">
+        <v>53.9</v>
+      </c>
+      <c r="M30">
+        <v>98.2</v>
+      </c>
+      <c r="N30">
+        <v>201.3</v>
+      </c>
+      <c r="O30">
+        <v>0.7146922183507549</v>
+      </c>
+      <c r="P30">
+        <v>0.5892062101929275</v>
+      </c>
+      <c r="Q30">
+        <v>0.6965162030951506</v>
+      </c>
+      <c r="R30">
+        <v>0.5269992997198879</v>
+      </c>
+      <c r="S30">
+        <v>38</v>
+      </c>
+      <c r="T30">
+        <v>81</v>
+      </c>
+      <c r="U30">
+        <v>88</v>
+      </c>
+      <c r="V30">
+        <v>210</v>
+      </c>
+      <c r="W30">
+        <v>3753</v>
+      </c>
+      <c r="X30">
+        <v>417</v>
+      </c>
+      <c r="Y30">
+        <v>10</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31">
+        <v>0.7</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>0.8001567375886525</v>
+      </c>
+      <c r="H31">
+        <v>0.7052491994105012</v>
+      </c>
+      <c r="I31">
+        <v>0.8764593833364508</v>
+      </c>
+      <c r="J31">
+        <v>0.590444545742925</v>
+      </c>
+      <c r="K31">
+        <v>12.7</v>
+      </c>
+      <c r="L31">
+        <v>62.3</v>
+      </c>
+      <c r="M31">
+        <v>89.8</v>
+      </c>
+      <c r="N31">
+        <v>210.5</v>
+      </c>
+      <c r="O31">
+        <v>0.690534262485482</v>
+      </c>
+      <c r="P31">
+        <v>0.5213082528620053</v>
+      </c>
+      <c r="Q31">
+        <v>0.7045238095238094</v>
+      </c>
+      <c r="R31">
+        <v>0.4179463755199049</v>
+      </c>
+      <c r="S31">
+        <v>31</v>
+      </c>
+      <c r="T31">
+        <v>98</v>
+      </c>
+      <c r="U31">
+        <v>71</v>
+      </c>
+      <c r="V31">
+        <v>217</v>
+      </c>
+      <c r="W31">
+        <v>3753</v>
+      </c>
+      <c r="X31">
+        <v>417</v>
+      </c>
+      <c r="Y31">
+        <v>10</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="A32">
+        <v>0.7</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32">
+        <v>0.7953638297872341</v>
+      </c>
+      <c r="H32">
+        <v>0.7067461526780672</v>
+      </c>
+      <c r="I32">
+        <v>0.8402944045854739</v>
+      </c>
+      <c r="J32">
+        <v>0.6113180292408845</v>
+      </c>
+      <c r="K32">
+        <v>17.8</v>
+      </c>
+      <c r="L32">
+        <v>59</v>
+      </c>
+      <c r="M32">
+        <v>93.09999999999999</v>
+      </c>
+      <c r="N32">
+        <v>205.4</v>
+      </c>
+      <c r="O32">
+        <v>0.7147502903600464</v>
+      </c>
+      <c r="P32">
+        <v>0.5718835591354765</v>
+      </c>
+      <c r="Q32">
+        <v>0.7249851455733809</v>
+      </c>
+      <c r="R32">
+        <v>0.4976533244876899</v>
+      </c>
+      <c r="S32">
+        <v>32</v>
+      </c>
+      <c r="T32">
+        <v>87</v>
+      </c>
+      <c r="U32">
+        <v>82</v>
+      </c>
+      <c r="V32">
+        <v>216</v>
+      </c>
+      <c r="W32">
+        <v>3753</v>
+      </c>
+      <c r="X32">
+        <v>417</v>
+      </c>
+      <c r="Y32">
+        <v>10</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix self edges error
</commit_message>
<xml_diff>
--- a/classifier/data/classifier_result/classifier_results.xlsx
+++ b/classifier/data/classifier_result/classifier_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="35">
   <si>
     <t>Correlation threshold</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>KFold k=10</t>
+  </si>
+  <si>
+    <t>adj_matrix_and_add= 2,</t>
+  </si>
+  <si>
+    <t>adj_matrix_and_add= 2,weigted_randomwalk</t>
+  </si>
+  <si>
+    <t>adj_matrix_and_add= 2,rw_on_main_graph</t>
+  </si>
+  <si>
+    <t>power_graph= 2,</t>
+  </si>
+  <si>
+    <t>power_graph= 2,weigted_randomwalk</t>
+  </si>
+  <si>
+    <t>power_graph= 2,rw_on_main_graph</t>
   </si>
   <si>
     <t>{'vector_size': 10, 'window_size': 2, 'learning_rate': 0.025, 'min_learning_rate': 0.001, 'min_count': 1, 'min_vocab_size': 'None', 'workers': 4, 'epochs': 50}</t>
@@ -458,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,52 +582,52 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.9549659574468086</v>
+        <v>0.9685617021276597</v>
       </c>
       <c r="H2">
-        <v>0.9471072523296737</v>
+        <v>0.9624199513908657</v>
       </c>
       <c r="I2">
-        <v>0.9007742182897068</v>
+        <v>0.9299466882757015</v>
       </c>
       <c r="J2">
-        <v>0.9986528168375216</v>
+        <v>0.9973595921696201</v>
       </c>
       <c r="K2">
-        <v>16.7</v>
+        <v>11.4</v>
       </c>
       <c r="L2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M2">
-        <v>151</v>
+        <v>150.8</v>
       </c>
       <c r="N2">
-        <v>207.4</v>
+        <v>212.7</v>
       </c>
       <c r="O2">
-        <v>0.6549361207897793</v>
+        <v>0.6713124274099883</v>
       </c>
       <c r="P2">
-        <v>0.5774825080920742</v>
+        <v>0.5680881592793952</v>
       </c>
       <c r="Q2">
-        <v>0.5696061343197567</v>
+        <v>0.603710587657956</v>
       </c>
       <c r="R2">
-        <v>0.6090307486631016</v>
+        <v>0.547084656399672</v>
       </c>
       <c r="S2">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="T2">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="U2">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="V2">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="W2">
         <v>3753</v>
@@ -621,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="Z2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -644,52 +662,52 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.9762879432624114</v>
+        <v>0.9666964539007094</v>
       </c>
       <c r="H3">
-        <v>0.9713338036289857</v>
+        <v>0.9604080467017271</v>
       </c>
       <c r="I3">
-        <v>0.9491211962917578</v>
+        <v>0.9239235258287628</v>
       </c>
       <c r="J3">
-        <v>0.9947217154380151</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>8.1</v>
+        <v>12.5</v>
       </c>
       <c r="L3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>150.4</v>
+        <v>151.2</v>
       </c>
       <c r="N3">
-        <v>216</v>
+        <v>211.6</v>
       </c>
       <c r="O3">
-        <v>0.6163182346109174</v>
+        <v>0.6351335656213705</v>
       </c>
       <c r="P3">
-        <v>0.5227341612635731</v>
+        <v>0.5414214800421696</v>
       </c>
       <c r="Q3">
-        <v>0.5209175546675546</v>
+        <v>0.5410996450155489</v>
       </c>
       <c r="R3">
-        <v>0.5353267973856209</v>
+        <v>0.5494139194139194</v>
       </c>
       <c r="S3">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="T3">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="U3">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="V3">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="W3">
         <v>3753</v>
@@ -701,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="Z3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -724,52 +742,52 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.9435120567375886</v>
+        <v>0.9499099290780142</v>
       </c>
       <c r="H4">
-        <v>0.9335826728297454</v>
+        <v>0.9348422405033204</v>
       </c>
       <c r="I4">
-        <v>0.8885907778343671</v>
+        <v>0.981826859326229</v>
       </c>
       <c r="J4">
-        <v>0.9834770857411999</v>
+        <v>0.8921884979885167</v>
       </c>
       <c r="K4">
-        <v>18.7</v>
+        <v>2.5</v>
       </c>
       <c r="L4">
-        <v>2.5</v>
+        <v>16.3</v>
       </c>
       <c r="M4">
-        <v>148.7</v>
+        <v>134.9</v>
       </c>
       <c r="N4">
-        <v>205.4</v>
+        <v>221.6</v>
       </c>
       <c r="O4">
-        <v>0.6906504065040651</v>
+        <v>0.6735772357723577</v>
       </c>
       <c r="P4">
-        <v>0.6142368341348836</v>
+        <v>0.5646260960757331</v>
       </c>
       <c r="Q4">
-        <v>0.6215732345569808</v>
+        <v>0.595059883357097</v>
       </c>
       <c r="R4">
-        <v>0.6249287485819994</v>
+        <v>0.5457111528822055</v>
       </c>
       <c r="S4">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="T4">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="U4">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="V4">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="W4">
         <v>3753</v>
@@ -781,7 +799,7 @@
         <v>10</v>
       </c>
       <c r="Z4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -804,52 +822,52 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.9618964539007093</v>
+        <v>0.9674964539007093</v>
       </c>
       <c r="H5">
-        <v>0.9546177934963953</v>
+        <v>0.9612691176147796</v>
       </c>
       <c r="I5">
-        <v>0.9195549938139918</v>
+        <v>0.9272658584423225</v>
       </c>
       <c r="J5">
-        <v>0.992700416666376</v>
+        <v>0.9979998210130659</v>
       </c>
       <c r="K5">
-        <v>13.2</v>
+        <v>11.9</v>
       </c>
       <c r="L5">
-        <v>1.1</v>
+        <v>0.3</v>
       </c>
       <c r="M5">
-        <v>150.1</v>
+        <v>150.9</v>
       </c>
       <c r="N5">
-        <v>210.9</v>
+        <v>212.2</v>
       </c>
       <c r="O5">
-        <v>0.6933797909407665</v>
+        <v>0.6260162601626016</v>
       </c>
       <c r="P5">
-        <v>0.6112872255714732</v>
+        <v>0.5220076429715899</v>
       </c>
       <c r="Q5">
-        <v>0.6223140417934468</v>
+        <v>0.5378140864982971</v>
       </c>
       <c r="R5">
-        <v>0.6120331560424439</v>
+        <v>0.5185654756320391</v>
       </c>
       <c r="S5">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="T5">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="U5">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="V5">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="W5">
         <v>3753</v>
@@ -861,7 +879,7 @@
         <v>10</v>
       </c>
       <c r="Z5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -884,49 +902,49 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.9611014184397163</v>
+        <v>0.9712226950354612</v>
       </c>
       <c r="H6">
-        <v>0.9530565429654831</v>
+        <v>0.9649977911157219</v>
       </c>
       <c r="I6">
-        <v>0.9281497258103372</v>
+        <v>0.9489160177908008</v>
       </c>
       <c r="J6">
-        <v>0.9794590846939017</v>
+        <v>0.9820006613226061</v>
       </c>
       <c r="K6">
-        <v>11.5</v>
+        <v>8.1</v>
       </c>
       <c r="L6">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="M6">
-        <v>148.1</v>
+        <v>148.5</v>
       </c>
       <c r="N6">
-        <v>212.6</v>
+        <v>216</v>
       </c>
       <c r="O6">
-        <v>0.6837398373983739</v>
+        <v>0.6277003484320558</v>
       </c>
       <c r="P6">
-        <v>0.6036872193980756</v>
+        <v>0.4985771262137546</v>
       </c>
       <c r="Q6">
-        <v>0.5937577463815854</v>
+        <v>0.5269978632478634</v>
       </c>
       <c r="R6">
-        <v>0.6251916556096122</v>
+        <v>0.486147504456328</v>
       </c>
       <c r="S6">
         <v>70</v>
       </c>
       <c r="T6">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="U6">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="V6">
         <v>179</v>
@@ -941,7 +959,7 @@
         <v>10</v>
       </c>
       <c r="Z6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -964,52 +982,52 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.9800134751773049</v>
+        <v>0.9632283687943263</v>
       </c>
       <c r="H7">
-        <v>0.9756232698061209</v>
+        <v>0.9524142491902825</v>
       </c>
       <c r="I7">
-        <v>0.9597754047813574</v>
+        <v>0.9950471061470182</v>
       </c>
       <c r="J7">
-        <v>0.992032597564017</v>
+        <v>0.9134466952379464</v>
       </c>
       <c r="K7">
-        <v>6.3</v>
+        <v>0.7</v>
       </c>
       <c r="L7">
-        <v>1.2</v>
+        <v>13.1</v>
       </c>
       <c r="M7">
-        <v>150</v>
+        <v>138.1</v>
       </c>
       <c r="N7">
-        <v>217.8</v>
+        <v>223.4</v>
       </c>
       <c r="O7">
-        <v>0.6619628339140533</v>
+        <v>0.5707897793263647</v>
       </c>
       <c r="P7">
-        <v>0.5530148132049756</v>
+        <v>0.4430653352274598</v>
       </c>
       <c r="Q7">
-        <v>0.6066154970760234</v>
+        <v>0.4759163273946556</v>
       </c>
       <c r="R7">
-        <v>0.5434403913080385</v>
+        <v>0.4328409258440218</v>
       </c>
       <c r="S7">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="T7">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="U7">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="V7">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="W7">
         <v>3753</v>
@@ -1021,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="Z7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1044,52 +1062,52 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0.9781468085106384</v>
+        <v>0.9786829787234043</v>
       </c>
       <c r="H8">
-        <v>0.9737268013621044</v>
+        <v>0.9741410892658815</v>
       </c>
       <c r="I8">
-        <v>0.9489480801959514</v>
+        <v>0.9546066863734796</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0.9946620157776993</v>
       </c>
       <c r="K8">
-        <v>8.199999999999999</v>
+        <v>7.2</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M8">
-        <v>151.2</v>
+        <v>150.4</v>
       </c>
       <c r="N8">
-        <v>215.9</v>
+        <v>216.9</v>
       </c>
       <c r="O8">
-        <v>0.6620789779326364</v>
+        <v>0.6523809523809525</v>
       </c>
       <c r="P8">
-        <v>0.563134236453202</v>
+        <v>0.5509793646612334</v>
       </c>
       <c r="Q8">
-        <v>0.590145540733776</v>
+        <v>0.5905350102254128</v>
       </c>
       <c r="R8">
-        <v>0.5436383460880364</v>
+        <v>0.5341992802519118</v>
       </c>
       <c r="S8">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T8">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="U8">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V8">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="W8">
         <v>3753</v>
@@ -1101,7 +1119,7 @@
         <v>10</v>
       </c>
       <c r="Z8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1124,52 +1142,52 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.9664255319148938</v>
+        <v>0.9560347517730496</v>
       </c>
       <c r="H9">
-        <v>0.9596269731423412</v>
+        <v>0.947556049727124</v>
       </c>
       <c r="I9">
-        <v>0.9328583819499267</v>
+        <v>0.9119906139839985</v>
       </c>
       <c r="J9">
-        <v>0.9880668562077919</v>
+        <v>0.9861011107170292</v>
       </c>
       <c r="K9">
-        <v>10.8</v>
+        <v>14.4</v>
       </c>
       <c r="L9">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="M9">
-        <v>149.4</v>
+        <v>149.1</v>
       </c>
       <c r="N9">
-        <v>213.3</v>
+        <v>209.7</v>
       </c>
       <c r="O9">
-        <v>0.6519744483159116</v>
+        <v>0.6664343786295005</v>
       </c>
       <c r="P9">
-        <v>0.5419174625753573</v>
+        <v>0.5539349878893817</v>
       </c>
       <c r="Q9">
-        <v>0.5520183982683983</v>
+        <v>0.60891607876128</v>
       </c>
       <c r="R9">
-        <v>0.5543835239071813</v>
+        <v>0.5180072786690435</v>
       </c>
       <c r="S9">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="T9">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="U9">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="V9">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="W9">
         <v>3753</v>
@@ -1181,7 +1199,7 @@
         <v>10</v>
       </c>
       <c r="Z9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1204,52 +1222,52 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0.9610985815602838</v>
+        <v>0.9485751773049647</v>
       </c>
       <c r="H10">
-        <v>0.9540670858080131</v>
+        <v>0.9331266261716159</v>
       </c>
       <c r="I10">
-        <v>0.9128125505581398</v>
+        <v>0.9770299735106353</v>
       </c>
       <c r="J10">
-        <v>0.9993548387096773</v>
+        <v>0.8933429636905625</v>
       </c>
       <c r="K10">
-        <v>14.5</v>
+        <v>3.2</v>
       </c>
       <c r="L10">
-        <v>0.1</v>
+        <v>16.1</v>
       </c>
       <c r="M10">
-        <v>151.1</v>
+        <v>135.1</v>
       </c>
       <c r="N10">
-        <v>209.6</v>
+        <v>220.9</v>
       </c>
       <c r="O10">
-        <v>0.6599303135888501</v>
+        <v>0.616492450638792</v>
       </c>
       <c r="P10">
-        <v>0.5770939672742359</v>
+        <v>0.4961333266236072</v>
       </c>
       <c r="Q10">
-        <v>0.5827750257997936</v>
+        <v>0.5555003819709702</v>
       </c>
       <c r="R10">
-        <v>0.5848457966182424</v>
+        <v>0.4763817790508799</v>
       </c>
       <c r="S10">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T10">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="U10">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="V10">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="W10">
         <v>3753</v>
@@ -1261,7 +1279,7 @@
         <v>10</v>
       </c>
       <c r="Z10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -1284,49 +1302,49 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.9578978723404257</v>
+        <v>0.9544326241134753</v>
       </c>
       <c r="H11">
-        <v>0.9504254999265521</v>
+        <v>0.9463988092585437</v>
       </c>
       <c r="I11">
-        <v>0.9056606329374564</v>
+        <v>0.9016519644679887</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0.9960173683826762</v>
       </c>
       <c r="K11">
-        <v>15.8</v>
+        <v>16.5</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="M11">
-        <v>151.2</v>
+        <v>150.6</v>
       </c>
       <c r="N11">
-        <v>208.3</v>
+        <v>207.6</v>
       </c>
       <c r="O11">
-        <v>0.6378629500580719</v>
+        <v>0.640650406504065</v>
       </c>
       <c r="P11">
-        <v>0.5416575897221059</v>
+        <v>0.5469475909672404</v>
       </c>
       <c r="Q11">
-        <v>0.5582081205688018</v>
+        <v>0.5664437729453209</v>
       </c>
       <c r="R11">
-        <v>0.5390413108563263</v>
+        <v>0.5429942503317117</v>
       </c>
       <c r="S11">
         <v>73</v>
       </c>
       <c r="T11">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U11">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="V11">
         <v>176</v>
@@ -1341,7 +1359,7 @@
         <v>10</v>
       </c>
       <c r="Z11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -1364,52 +1382,52 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.9709567375886525</v>
+        <v>0.9704234042553193</v>
       </c>
       <c r="H12">
-        <v>0.9645802356594905</v>
+        <v>0.9644773233556021</v>
       </c>
       <c r="I12">
-        <v>0.947727464466696</v>
+        <v>0.9368335500730478</v>
       </c>
       <c r="J12">
-        <v>0.9820998783390669</v>
+        <v>0.9939932965849125</v>
       </c>
       <c r="K12">
-        <v>8.199999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="L12">
-        <v>2.7</v>
+        <v>0.9</v>
       </c>
       <c r="M12">
-        <v>148.5</v>
+        <v>150.3</v>
       </c>
       <c r="N12">
-        <v>215.9</v>
+        <v>213.9</v>
       </c>
       <c r="O12">
-        <v>0.6451219512195122</v>
+        <v>0.6212543554006968</v>
       </c>
       <c r="P12">
-        <v>0.54236839588287</v>
+        <v>0.5352507193735553</v>
       </c>
       <c r="Q12">
-        <v>0.5489909600203717</v>
+        <v>0.5381792016892636</v>
       </c>
       <c r="R12">
-        <v>0.5553317734896682</v>
+        <v>0.5559450271950273</v>
       </c>
       <c r="S12">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="T12">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U12">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="V12">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="W12">
         <v>3753</v>
@@ -1421,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="Z12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -1441,68 +1459,3747 @@
         <v>27</v>
       </c>
       <c r="F13">
-        <f> ,weigted_randomwalk</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.9832163120567377</v>
+        <v>0.9456432624113476</v>
       </c>
       <c r="H13">
-        <v>0.9794305511685536</v>
+        <v>0.930781344708117</v>
       </c>
       <c r="I13">
-        <v>0.9697251322734489</v>
+        <v>0.9555783168085</v>
       </c>
       <c r="J13">
-        <v>0.989411228730094</v>
+        <v>0.9073902150243944</v>
       </c>
       <c r="K13">
-        <v>4.7</v>
+        <v>6.4</v>
       </c>
       <c r="L13">
+        <v>14</v>
+      </c>
+      <c r="M13">
+        <v>137.2</v>
+      </c>
+      <c r="N13">
+        <v>217.7</v>
+      </c>
+      <c r="O13">
+        <v>0.6211962833914052</v>
+      </c>
+      <c r="P13">
+        <v>0.4998352108922677</v>
+      </c>
+      <c r="Q13">
+        <v>0.5581594304388422</v>
+      </c>
+      <c r="R13">
+        <v>0.4775833531793284</v>
+      </c>
+      <c r="S13">
+        <v>69</v>
+      </c>
+      <c r="T13">
+        <v>89</v>
+      </c>
+      <c r="U13">
+        <v>79</v>
+      </c>
+      <c r="V13">
+        <v>180</v>
+      </c>
+      <c r="W13">
+        <v>3753</v>
+      </c>
+      <c r="X13">
+        <v>417</v>
+      </c>
+      <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14">
+        <v>0.7</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.9579063829787234</v>
+      </c>
+      <c r="H14">
+        <v>0.9507741505148386</v>
+      </c>
+      <c r="I14">
+        <v>0.9064141448517609</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>15.8</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>151.2</v>
+      </c>
+      <c r="N14">
+        <v>208.3</v>
+      </c>
+      <c r="O14">
+        <v>0.6524970963995353</v>
+      </c>
+      <c r="P14">
+        <v>0.5643817118168464</v>
+      </c>
+      <c r="Q14">
+        <v>0.5621275637361248</v>
+      </c>
+      <c r="R14">
+        <v>0.5902822341057636</v>
+      </c>
+      <c r="S14">
+        <v>76</v>
+      </c>
+      <c r="T14">
+        <v>69</v>
+      </c>
+      <c r="U14">
+        <v>99</v>
+      </c>
+      <c r="V14">
+        <v>173</v>
+      </c>
+      <c r="W14">
+        <v>3753</v>
+      </c>
+      <c r="X14">
+        <v>417</v>
+      </c>
+      <c r="Y14">
+        <v>10</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15">
+        <v>0.7</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.978686524822695</v>
+      </c>
+      <c r="H15">
+        <v>0.9743713002172797</v>
+      </c>
+      <c r="I15">
+        <v>0.9512950355495633</v>
+      </c>
+      <c r="J15">
+        <v>0.9986881720430107</v>
+      </c>
+      <c r="K15">
+        <v>7.8</v>
+      </c>
+      <c r="L15">
+        <v>0.2</v>
+      </c>
+      <c r="M15">
+        <v>151</v>
+      </c>
+      <c r="N15">
+        <v>216.3</v>
+      </c>
+      <c r="O15">
+        <v>0.6401277584204413</v>
+      </c>
+      <c r="P15">
+        <v>0.5430459336479082</v>
+      </c>
+      <c r="Q15">
+        <v>0.556909110355402</v>
+      </c>
+      <c r="R15">
+        <v>0.5449160756833391</v>
+      </c>
+      <c r="S15">
+        <v>74</v>
+      </c>
+      <c r="T15">
+        <v>76</v>
+      </c>
+      <c r="U15">
+        <v>92</v>
+      </c>
+      <c r="V15">
+        <v>175</v>
+      </c>
+      <c r="W15">
+        <v>3753</v>
+      </c>
+      <c r="X15">
+        <v>417</v>
+      </c>
+      <c r="Y15">
+        <v>10</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16">
+        <v>0.7</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0.9589631205673761</v>
+      </c>
+      <c r="H16">
+        <v>0.9466053995237502</v>
+      </c>
+      <c r="I16">
+        <v>0.9906609274360653</v>
+      </c>
+      <c r="J16">
+        <v>0.9064658200241604</v>
+      </c>
+      <c r="K16">
+        <v>1.3</v>
+      </c>
+      <c r="L16">
+        <v>14.1</v>
+      </c>
+      <c r="M16">
+        <v>137.1</v>
+      </c>
+      <c r="N16">
+        <v>222.8</v>
+      </c>
+      <c r="O16">
+        <v>0.6188153310104529</v>
+      </c>
+      <c r="P16">
+        <v>0.4833657936471003</v>
+      </c>
+      <c r="Q16">
+        <v>0.5305754049871697</v>
+      </c>
+      <c r="R16">
+        <v>0.4578484166332463</v>
+      </c>
+      <c r="S16">
+        <v>67</v>
+      </c>
+      <c r="T16">
+        <v>92</v>
+      </c>
+      <c r="U16">
+        <v>76</v>
+      </c>
+      <c r="V16">
+        <v>182</v>
+      </c>
+      <c r="W16">
+        <v>3753</v>
+      </c>
+      <c r="X16">
+        <v>417</v>
+      </c>
+      <c r="Y16">
+        <v>10</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17">
+        <v>0.7</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0.9629609929078015</v>
+      </c>
+      <c r="H17">
+        <v>0.9556787693355602</v>
+      </c>
+      <c r="I17">
+        <v>0.9272771694966349</v>
+      </c>
+      <c r="J17">
+        <v>0.9861253990827372</v>
+      </c>
+      <c r="K17">
+        <v>11.8</v>
+      </c>
+      <c r="L17">
+        <v>2.1</v>
+      </c>
+      <c r="M17">
+        <v>149.1</v>
+      </c>
+      <c r="N17">
+        <v>212.3</v>
+      </c>
+      <c r="O17">
+        <v>0.6689314750290359</v>
+      </c>
+      <c r="P17">
+        <v>0.5774562790691823</v>
+      </c>
+      <c r="Q17">
+        <v>0.6061193424738316</v>
+      </c>
+      <c r="R17">
+        <v>0.5772848032600354</v>
+      </c>
+      <c r="S17">
+        <v>66</v>
+      </c>
+      <c r="T17">
+        <v>72</v>
+      </c>
+      <c r="U17">
+        <v>96</v>
+      </c>
+      <c r="V17">
+        <v>183</v>
+      </c>
+      <c r="W17">
+        <v>3753</v>
+      </c>
+      <c r="X17">
+        <v>417</v>
+      </c>
+      <c r="Y17">
+        <v>10</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18">
+        <v>0.7</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0.9613617021276596</v>
+      </c>
+      <c r="H18">
+        <v>0.9542740313568382</v>
+      </c>
+      <c r="I18">
+        <v>0.9143888260382719</v>
+      </c>
+      <c r="J18">
+        <v>0.9979683148427156</v>
+      </c>
+      <c r="K18">
+        <v>14.2</v>
+      </c>
+      <c r="L18">
+        <v>0.3</v>
+      </c>
+      <c r="M18">
+        <v>150.9</v>
+      </c>
+      <c r="N18">
+        <v>209.9</v>
+      </c>
+      <c r="O18">
+        <v>0.6617305458768872</v>
+      </c>
+      <c r="P18">
+        <v>0.5674222033523907</v>
+      </c>
+      <c r="Q18">
+        <v>0.5874690924307292</v>
+      </c>
+      <c r="R18">
+        <v>0.5622210078363329</v>
+      </c>
+      <c r="S18">
+        <v>67</v>
+      </c>
+      <c r="T18">
+        <v>74</v>
+      </c>
+      <c r="U18">
+        <v>94</v>
+      </c>
+      <c r="V18">
+        <v>182</v>
+      </c>
+      <c r="W18">
+        <v>3753</v>
+      </c>
+      <c r="X18">
+        <v>417</v>
+      </c>
+      <c r="Y18">
+        <v>10</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19">
+        <v>0.7</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0.9475028368794327</v>
+      </c>
+      <c r="H19">
+        <v>0.931424647789308</v>
+      </c>
+      <c r="I19">
+        <v>0.9838764204277355</v>
+      </c>
+      <c r="J19">
+        <v>0.8843601227718871</v>
+      </c>
+      <c r="K19">
+        <v>2.2</v>
+      </c>
+      <c r="L19">
+        <v>17.5</v>
+      </c>
+      <c r="M19">
+        <v>133.7</v>
+      </c>
+      <c r="N19">
+        <v>221.9</v>
+      </c>
+      <c r="O19">
+        <v>0.6333914053426248</v>
+      </c>
+      <c r="P19">
+        <v>0.5243645629437849</v>
+      </c>
+      <c r="Q19">
+        <v>0.5452062643239114</v>
+      </c>
+      <c r="R19">
+        <v>0.5184980267410608</v>
+      </c>
+      <c r="S19">
+        <v>71</v>
+      </c>
+      <c r="T19">
+        <v>82</v>
+      </c>
+      <c r="U19">
+        <v>86</v>
+      </c>
+      <c r="V19">
+        <v>178</v>
+      </c>
+      <c r="W19">
+        <v>3753</v>
+      </c>
+      <c r="X19">
+        <v>417</v>
+      </c>
+      <c r="Y19">
+        <v>10</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20">
+        <v>0.7</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0.9563007092198582</v>
+      </c>
+      <c r="H20">
+        <v>0.9484151817617331</v>
+      </c>
+      <c r="I20">
+        <v>0.9047018759196105</v>
+      </c>
+      <c r="J20">
+        <v>0.9966742304123966</v>
+      </c>
+      <c r="K20">
+        <v>15.9</v>
+      </c>
+      <c r="L20">
+        <v>0.5</v>
+      </c>
+      <c r="M20">
+        <v>150.7</v>
+      </c>
+      <c r="N20">
+        <v>208.2</v>
+      </c>
+      <c r="O20">
+        <v>0.6957607433217189</v>
+      </c>
+      <c r="P20">
+        <v>0.6242893807428691</v>
+      </c>
+      <c r="Q20">
+        <v>0.6237103797475315</v>
+      </c>
+      <c r="R20">
+        <v>0.6372299621603027</v>
+      </c>
+      <c r="S20">
+        <v>65</v>
+      </c>
+      <c r="T20">
+        <v>62</v>
+      </c>
+      <c r="U20">
+        <v>106</v>
+      </c>
+      <c r="V20">
+        <v>184</v>
+      </c>
+      <c r="W20">
+        <v>3753</v>
+      </c>
+      <c r="X20">
+        <v>417</v>
+      </c>
+      <c r="Y20">
+        <v>10</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21">
+        <v>0.7</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0.9624333333333335</v>
+      </c>
+      <c r="H21">
+        <v>0.9551457367575447</v>
+      </c>
+      <c r="I21">
+        <v>0.9221796000323048</v>
+      </c>
+      <c r="J21">
+        <v>0.9907593155046719</v>
+      </c>
+      <c r="K21">
+        <v>12.7</v>
+      </c>
+      <c r="L21">
+        <v>1.4</v>
+      </c>
+      <c r="M21">
+        <v>149.8</v>
+      </c>
+      <c r="N21">
+        <v>211.4</v>
+      </c>
+      <c r="O21">
+        <v>0.6260162601626015</v>
+      </c>
+      <c r="P21">
+        <v>0.5164570884689732</v>
+      </c>
+      <c r="Q21">
+        <v>0.5417215219421101</v>
+      </c>
+      <c r="R21">
+        <v>0.5042269701402829</v>
+      </c>
+      <c r="S21">
+        <v>73</v>
+      </c>
+      <c r="T21">
+        <v>83</v>
+      </c>
+      <c r="U21">
+        <v>85</v>
+      </c>
+      <c r="V21">
+        <v>176</v>
+      </c>
+      <c r="W21">
+        <v>3753</v>
+      </c>
+      <c r="X21">
+        <v>417</v>
+      </c>
+      <c r="Y21">
+        <v>10</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22">
+        <v>0.7</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0.9443085106382979</v>
+      </c>
+      <c r="H22">
+        <v>0.9269647052388027</v>
+      </c>
+      <c r="I22">
+        <v>0.9809908917111221</v>
+      </c>
+      <c r="J22">
+        <v>0.8789058819677397</v>
+      </c>
+      <c r="K22">
+        <v>2.6</v>
+      </c>
+      <c r="L22">
+        <v>18.3</v>
+      </c>
+      <c r="M22">
+        <v>132.9</v>
+      </c>
+      <c r="N22">
+        <v>221.5</v>
+      </c>
+      <c r="O22">
+        <v>0.6544715447154471</v>
+      </c>
+      <c r="P22">
+        <v>0.5253070997418823</v>
+      </c>
+      <c r="Q22">
+        <v>0.5775233426704015</v>
+      </c>
+      <c r="R22">
+        <v>0.4904045954045954</v>
+      </c>
+      <c r="S22">
+        <v>59</v>
+      </c>
+      <c r="T22">
+        <v>85</v>
+      </c>
+      <c r="U22">
+        <v>83</v>
+      </c>
+      <c r="V22">
+        <v>190</v>
+      </c>
+      <c r="W22">
+        <v>3753</v>
+      </c>
+      <c r="X22">
+        <v>417</v>
+      </c>
+      <c r="Y22">
+        <v>10</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23">
+        <v>0.7</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0.9800156028368795</v>
+      </c>
+      <c r="H23">
+        <v>0.9756992586222865</v>
+      </c>
+      <c r="I23">
+        <v>0.9562712514910411</v>
+      </c>
+      <c r="J23">
+        <v>0.9959949946155137</v>
+      </c>
+      <c r="K23">
+        <v>6.9</v>
+      </c>
+      <c r="L23">
+        <v>0.6</v>
+      </c>
+      <c r="M23">
+        <v>150.6</v>
+      </c>
+      <c r="N23">
+        <v>217.2</v>
+      </c>
+      <c r="O23">
+        <v>0.6067363530778165</v>
+      </c>
+      <c r="P23">
+        <v>0.4628276042981925</v>
+      </c>
+      <c r="Q23">
+        <v>0.5046476072946662</v>
+      </c>
+      <c r="R23">
+        <v>0.4376841613838519</v>
+      </c>
+      <c r="S23">
+        <v>70</v>
+      </c>
+      <c r="T23">
+        <v>94</v>
+      </c>
+      <c r="U23">
+        <v>74</v>
+      </c>
+      <c r="V23">
+        <v>179</v>
+      </c>
+      <c r="W23">
+        <v>3753</v>
+      </c>
+      <c r="X23">
+        <v>417</v>
+      </c>
+      <c r="Y23">
+        <v>10</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24">
+        <v>0.7</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0.9728156028368795</v>
+      </c>
+      <c r="H24">
+        <v>0.967194789258814</v>
+      </c>
+      <c r="I24">
+        <v>0.9455020071485866</v>
+      </c>
+      <c r="J24">
+        <v>0.9900642438464711</v>
+      </c>
+      <c r="K24">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="L24">
+        <v>1.5</v>
+      </c>
+      <c r="M24">
+        <v>149.7</v>
+      </c>
+      <c r="N24">
+        <v>215.4</v>
+      </c>
+      <c r="O24">
+        <v>0.6788037166085945</v>
+      </c>
+      <c r="P24">
+        <v>0.5822292289864446</v>
+      </c>
+      <c r="Q24">
+        <v>0.6191397233657296</v>
+      </c>
+      <c r="R24">
+        <v>0.5813290802764487</v>
+      </c>
+      <c r="S24">
+        <v>63</v>
+      </c>
+      <c r="T24">
+        <v>71</v>
+      </c>
+      <c r="U24">
+        <v>97</v>
+      </c>
+      <c r="V24">
+        <v>186</v>
+      </c>
+      <c r="W24">
+        <v>3753</v>
+      </c>
+      <c r="X24">
+        <v>417</v>
+      </c>
+      <c r="Y24">
+        <v>10</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25">
+        <v>0.7</v>
+      </c>
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0.9768156028368795</v>
+      </c>
+      <c r="H25">
+        <v>0.9708246973793002</v>
+      </c>
+      <c r="I25">
+        <v>0.9824837069435975</v>
+      </c>
+      <c r="J25">
+        <v>0.9595738938618894</v>
+      </c>
+      <c r="K25">
+        <v>2.6</v>
+      </c>
+      <c r="L25">
+        <v>6.1</v>
+      </c>
+      <c r="M25">
+        <v>145.1</v>
+      </c>
+      <c r="N25">
+        <v>221.5</v>
+      </c>
+      <c r="O25">
+        <v>0.606794425087108</v>
+      </c>
+      <c r="P25">
+        <v>0.4489384757119311</v>
+      </c>
+      <c r="Q25">
+        <v>0.5025954592363261</v>
+      </c>
+      <c r="R25">
+        <v>0.4119964787534448</v>
+      </c>
+      <c r="S25">
+        <v>68</v>
+      </c>
+      <c r="T25">
+        <v>96</v>
+      </c>
+      <c r="U25">
+        <v>72</v>
+      </c>
+      <c r="V25">
+        <v>181</v>
+      </c>
+      <c r="W25">
+        <v>3753</v>
+      </c>
+      <c r="X25">
+        <v>417</v>
+      </c>
+      <c r="Y25">
+        <v>10</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26">
+        <v>0.7</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0.9698900709219858</v>
+      </c>
+      <c r="H26">
+        <v>0.9641130562473326</v>
+      </c>
+      <c r="I26">
+        <v>0.9308414912843812</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>11.3</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>151.2</v>
+      </c>
+      <c r="N26">
+        <v>212.8</v>
+      </c>
+      <c r="O26">
+        <v>0.638095238095238</v>
+      </c>
+      <c r="P26">
+        <v>0.5670683764688874</v>
+      </c>
+      <c r="Q26">
+        <v>0.5576470588235295</v>
+      </c>
+      <c r="R26">
+        <v>0.5990552584670231</v>
+      </c>
+      <c r="S26">
+        <v>83</v>
+      </c>
+      <c r="T26">
+        <v>68</v>
+      </c>
+      <c r="U26">
+        <v>100</v>
+      </c>
+      <c r="V26">
+        <v>166</v>
+      </c>
+      <c r="W26">
+        <v>3753</v>
+      </c>
+      <c r="X26">
+        <v>417</v>
+      </c>
+      <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27">
+        <v>0.7</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0.9794815602836879</v>
+      </c>
+      <c r="H27">
+        <v>0.9750461774505194</v>
+      </c>
+      <c r="I27">
+        <v>0.9581286183381919</v>
+      </c>
+      <c r="J27">
+        <v>0.9926876260860962</v>
+      </c>
+      <c r="K27">
+        <v>6.6</v>
+      </c>
+      <c r="L27">
+        <v>1.1</v>
+      </c>
+      <c r="M27">
+        <v>150.1</v>
+      </c>
+      <c r="N27">
+        <v>217.5</v>
+      </c>
+      <c r="O27">
+        <v>0.6354819976771195</v>
+      </c>
+      <c r="P27">
+        <v>0.5370562770562771</v>
+      </c>
+      <c r="Q27">
+        <v>0.5479480942174442</v>
+      </c>
+      <c r="R27">
+        <v>0.5353661727849034</v>
+      </c>
+      <c r="S27">
+        <v>74</v>
+      </c>
+      <c r="T27">
+        <v>78</v>
+      </c>
+      <c r="U27">
+        <v>90</v>
+      </c>
+      <c r="V27">
+        <v>175</v>
+      </c>
+      <c r="W27">
+        <v>3753</v>
+      </c>
+      <c r="X27">
+        <v>417</v>
+      </c>
+      <c r="Y27">
+        <v>10</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28">
+        <v>0.7</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0.9432425531914894</v>
+      </c>
+      <c r="H28">
+        <v>0.9258780965191358</v>
+      </c>
+      <c r="I28">
+        <v>0.9730552375377253</v>
+      </c>
+      <c r="J28">
+        <v>0.883358035818867</v>
+      </c>
+      <c r="K28">
+        <v>3.7</v>
+      </c>
+      <c r="L28">
+        <v>17.6</v>
+      </c>
+      <c r="M28">
+        <v>133.6</v>
+      </c>
+      <c r="N28">
+        <v>220.4</v>
+      </c>
+      <c r="O28">
+        <v>0.6307200929152148</v>
+      </c>
+      <c r="P28">
+        <v>0.4730013403834915</v>
+      </c>
+      <c r="Q28">
+        <v>0.5446750360063054</v>
+      </c>
+      <c r="R28">
+        <v>0.4451046176046176</v>
+      </c>
+      <c r="S28">
+        <v>60</v>
+      </c>
+      <c r="T28">
+        <v>94</v>
+      </c>
+      <c r="U28">
+        <v>74</v>
+      </c>
+      <c r="V28">
+        <v>189</v>
+      </c>
+      <c r="W28">
+        <v>3753</v>
+      </c>
+      <c r="X28">
+        <v>417</v>
+      </c>
+      <c r="Y28">
+        <v>10</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29">
+        <v>0.7</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0.9381886524822693</v>
+      </c>
+      <c r="H29">
+        <v>0.928347441766849</v>
+      </c>
+      <c r="I29">
+        <v>0.8718291138853189</v>
+      </c>
+      <c r="J29">
+        <v>0.9928128956318002</v>
+      </c>
+      <c r="K29">
+        <v>22.1</v>
+      </c>
+      <c r="L29">
+        <v>1.1</v>
+      </c>
+      <c r="M29">
+        <v>150.1</v>
+      </c>
+      <c r="N29">
+        <v>202</v>
+      </c>
+      <c r="O29">
+        <v>0.6736353077816492</v>
+      </c>
+      <c r="P29">
+        <v>0.6055887288145353</v>
+      </c>
+      <c r="Q29">
+        <v>0.5897245564892623</v>
+      </c>
+      <c r="R29">
+        <v>0.6394428528987353</v>
+      </c>
+      <c r="S29">
+        <v>74</v>
+      </c>
+      <c r="T29">
+        <v>62</v>
+      </c>
+      <c r="U29">
+        <v>106</v>
+      </c>
+      <c r="V29">
+        <v>175</v>
+      </c>
+      <c r="W29">
+        <v>3753</v>
+      </c>
+      <c r="X29">
+        <v>417</v>
+      </c>
+      <c r="Y29">
+        <v>10</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30">
+        <v>0.7</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0.9698943262411349</v>
+      </c>
+      <c r="H30">
+        <v>0.9638082420568411</v>
+      </c>
+      <c r="I30">
+        <v>0.9378954175928149</v>
+      </c>
+      <c r="J30">
+        <v>0.9913291952086201</v>
+      </c>
+      <c r="K30">
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <v>1.3</v>
+      </c>
+      <c r="M30">
+        <v>149.9</v>
+      </c>
+      <c r="N30">
+        <v>214.1</v>
+      </c>
+      <c r="O30">
+        <v>0.628397212543554</v>
+      </c>
+      <c r="P30">
+        <v>0.5421327606840394</v>
+      </c>
+      <c r="Q30">
+        <v>0.5350091360308078</v>
+      </c>
+      <c r="R30">
+        <v>0.5607393483709273</v>
+      </c>
+      <c r="S30">
+        <v>80</v>
+      </c>
+      <c r="T30">
+        <v>75</v>
+      </c>
+      <c r="U30">
+        <v>93</v>
+      </c>
+      <c r="V30">
+        <v>169</v>
+      </c>
+      <c r="W30">
+        <v>3753</v>
+      </c>
+      <c r="X30">
+        <v>417</v>
+      </c>
+      <c r="Y30">
+        <v>10</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31">
+        <v>0.7</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0.9400496453900707</v>
+      </c>
+      <c r="H31">
+        <v>0.9199652755796324</v>
+      </c>
+      <c r="I31">
+        <v>0.9931599050266534</v>
+      </c>
+      <c r="J31">
+        <v>0.8570538503211294</v>
+      </c>
+      <c r="K31">
+        <v>0.9</v>
+      </c>
+      <c r="L31">
+        <v>21.6</v>
+      </c>
+      <c r="M31">
+        <v>129.6</v>
+      </c>
+      <c r="N31">
+        <v>223.2</v>
+      </c>
+      <c r="O31">
+        <v>0.6451219512195121</v>
+      </c>
+      <c r="P31">
+        <v>0.4906482680907233</v>
+      </c>
+      <c r="Q31">
+        <v>0.5735301544860369</v>
+      </c>
+      <c r="R31">
+        <v>0.4447681987774866</v>
+      </c>
+      <c r="S31">
+        <v>54</v>
+      </c>
+      <c r="T31">
+        <v>94</v>
+      </c>
+      <c r="U31">
+        <v>74</v>
+      </c>
+      <c r="V31">
+        <v>195</v>
+      </c>
+      <c r="W31">
+        <v>3753</v>
+      </c>
+      <c r="X31">
+        <v>417</v>
+      </c>
+      <c r="Y31">
+        <v>10</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="A32">
+        <v>0.7</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0.9738900709219858</v>
+      </c>
+      <c r="H32">
+        <v>0.9683036038825008</v>
+      </c>
+      <c r="I32">
+        <v>0.9494469623023564</v>
+      </c>
+      <c r="J32">
+        <v>0.9880757321884879</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+      <c r="L32">
+        <v>1.8</v>
+      </c>
+      <c r="M32">
+        <v>149.4</v>
+      </c>
+      <c r="N32">
+        <v>216.1</v>
+      </c>
+      <c r="O32">
+        <v>0.6761324041811846</v>
+      </c>
+      <c r="P32">
+        <v>0.5946637465361816</v>
+      </c>
+      <c r="Q32">
+        <v>0.6006015904385469</v>
+      </c>
+      <c r="R32">
+        <v>0.6091691237898669</v>
+      </c>
+      <c r="S32">
+        <v>69</v>
+      </c>
+      <c r="T32">
+        <v>66</v>
+      </c>
+      <c r="U32">
+        <v>102</v>
+      </c>
+      <c r="V32">
+        <v>180</v>
+      </c>
+      <c r="W32">
+        <v>3753</v>
+      </c>
+      <c r="X32">
+        <v>417</v>
+      </c>
+      <c r="Y32">
+        <v>10</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
+      <c r="A33">
+        <v>0.7</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0.9722865248226951</v>
+      </c>
+      <c r="H33">
+        <v>0.9660813238756489</v>
+      </c>
+      <c r="I33">
+        <v>0.9545446614002</v>
+      </c>
+      <c r="J33">
+        <v>0.9780921995933175</v>
+      </c>
+      <c r="K33">
+        <v>7.1</v>
+      </c>
+      <c r="L33">
+        <v>3.3</v>
+      </c>
+      <c r="M33">
+        <v>147.9</v>
+      </c>
+      <c r="N33">
+        <v>217</v>
+      </c>
+      <c r="O33">
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="P33">
+        <v>0.5880079392460796</v>
+      </c>
+      <c r="Q33">
+        <v>0.6124401913875598</v>
+      </c>
+      <c r="R33">
+        <v>0.5796683497960587</v>
+      </c>
+      <c r="S33">
+        <v>63</v>
+      </c>
+      <c r="T33">
+        <v>71</v>
+      </c>
+      <c r="U33">
+        <v>97</v>
+      </c>
+      <c r="V33">
+        <v>186</v>
+      </c>
+      <c r="W33">
+        <v>3753</v>
+      </c>
+      <c r="X33">
+        <v>417</v>
+      </c>
+      <c r="Y33">
+        <v>10</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34">
+        <v>0.7</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0.9701602836879433</v>
+      </c>
+      <c r="H34">
+        <v>0.9620526695303562</v>
+      </c>
+      <c r="I34">
+        <v>0.9855756945833981</v>
+      </c>
+      <c r="J34">
+        <v>0.9397503751917426</v>
+      </c>
+      <c r="K34">
+        <v>2.1</v>
+      </c>
+      <c r="L34">
+        <v>9.1</v>
+      </c>
+      <c r="M34">
+        <v>142.1</v>
+      </c>
+      <c r="N34">
+        <v>222</v>
+      </c>
+      <c r="O34">
+        <v>0.6760162601626015</v>
+      </c>
+      <c r="P34">
+        <v>0.5618949730429807</v>
+      </c>
+      <c r="Q34">
+        <v>0.6181088278766297</v>
+      </c>
+      <c r="R34">
+        <v>0.535154804345981</v>
+      </c>
+      <c r="S34">
+        <v>57</v>
+      </c>
+      <c r="T34">
+        <v>78</v>
+      </c>
+      <c r="U34">
+        <v>90</v>
+      </c>
+      <c r="V34">
+        <v>192</v>
+      </c>
+      <c r="W34">
+        <v>3753</v>
+      </c>
+      <c r="X34">
+        <v>417</v>
+      </c>
+      <c r="Y34">
+        <v>10</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
+      <c r="A35">
+        <v>0.7</v>
+      </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35">
+        <v>0.9589666666666666</v>
+      </c>
+      <c r="H35">
+        <v>0.9511113106263567</v>
+      </c>
+      <c r="I35">
+        <v>0.9152300990532473</v>
+      </c>
+      <c r="J35">
+        <v>0.9900996026786878</v>
+      </c>
+      <c r="K35">
+        <v>13.9</v>
+      </c>
+      <c r="L35">
+        <v>1.5</v>
+      </c>
+      <c r="M35">
+        <v>149.7</v>
+      </c>
+      <c r="N35">
+        <v>210.2</v>
+      </c>
+      <c r="O35">
+        <v>0.6790940766550523</v>
+      </c>
+      <c r="P35">
+        <v>0.5969633280662693</v>
+      </c>
+      <c r="Q35">
+        <v>0.6069450350990599</v>
+      </c>
+      <c r="R35">
+        <v>0.5944201331004736</v>
+      </c>
+      <c r="S35">
+        <v>66</v>
+      </c>
+      <c r="T35">
+        <v>68</v>
+      </c>
+      <c r="U35">
+        <v>100</v>
+      </c>
+      <c r="V35">
+        <v>183</v>
+      </c>
+      <c r="W35">
+        <v>3753</v>
+      </c>
+      <c r="X35">
+        <v>417</v>
+      </c>
+      <c r="Y35">
+        <v>10</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
+      <c r="A36">
+        <v>0.7</v>
+      </c>
+      <c r="B36">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36">
+        <v>0.9547000000000001</v>
+      </c>
+      <c r="H36">
+        <v>0.946815301371986</v>
+      </c>
+      <c r="I36">
+        <v>0.8990558822109342</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>17</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>151.2</v>
+      </c>
+      <c r="N36">
+        <v>207.1</v>
+      </c>
+      <c r="O36">
+        <v>0.659698025551684</v>
+      </c>
+      <c r="P36">
+        <v>0.5764563851001696</v>
+      </c>
+      <c r="Q36">
+        <v>0.5741743877037995</v>
+      </c>
+      <c r="R36">
+        <v>0.5901275917065392</v>
+      </c>
+      <c r="S36">
+        <v>73</v>
+      </c>
+      <c r="T36">
+        <v>69</v>
+      </c>
+      <c r="U36">
+        <v>99</v>
+      </c>
+      <c r="V36">
+        <v>176</v>
+      </c>
+      <c r="W36">
+        <v>3753</v>
+      </c>
+      <c r="X36">
+        <v>417</v>
+      </c>
+      <c r="Y36">
+        <v>10</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
+      <c r="A37">
+        <v>0.7</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>0.9477744680851063</v>
+      </c>
+      <c r="H37">
+        <v>0.9309691694831761</v>
+      </c>
+      <c r="I37">
+        <v>0.9939601120073078</v>
+      </c>
+      <c r="J37">
+        <v>0.8755346276153656</v>
+      </c>
+      <c r="K37">
+        <v>0.8</v>
+      </c>
+      <c r="L37">
+        <v>18.8</v>
+      </c>
+      <c r="M37">
+        <v>132.4</v>
+      </c>
+      <c r="N37">
+        <v>223.3</v>
+      </c>
+      <c r="O37">
+        <v>0.6644018583042972</v>
+      </c>
+      <c r="P37">
+        <v>0.5353556505600443</v>
+      </c>
+      <c r="Q37">
+        <v>0.6020691589112641</v>
+      </c>
+      <c r="R37">
+        <v>0.4935902198936254</v>
+      </c>
+      <c r="S37">
+        <v>55</v>
+      </c>
+      <c r="T37">
+        <v>85</v>
+      </c>
+      <c r="U37">
+        <v>83</v>
+      </c>
+      <c r="V37">
+        <v>194</v>
+      </c>
+      <c r="W37">
+        <v>3753</v>
+      </c>
+      <c r="X37">
+        <v>417</v>
+      </c>
+      <c r="Y37">
+        <v>10</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26">
+      <c r="A38">
+        <v>0.7</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38">
+        <v>0.9650936170212768</v>
+      </c>
+      <c r="H38">
+        <v>0.9585596707860274</v>
+      </c>
+      <c r="I38">
+        <v>0.922266469168736</v>
+      </c>
+      <c r="J38">
+        <v>0.9979901984351149</v>
+      </c>
+      <c r="K38">
+        <v>12.8</v>
+      </c>
+      <c r="L38">
+        <v>0.3</v>
+      </c>
+      <c r="M38">
+        <v>150.9</v>
+      </c>
+      <c r="N38">
+        <v>211.3</v>
+      </c>
+      <c r="O38">
+        <v>0.6665505226480837</v>
+      </c>
+      <c r="P38">
+        <v>0.5709017646871573</v>
+      </c>
+      <c r="Q38">
+        <v>0.5852887072507815</v>
+      </c>
+      <c r="R38">
+        <v>0.5639581752433415</v>
+      </c>
+      <c r="S38">
+        <v>66</v>
+      </c>
+      <c r="T38">
+        <v>73</v>
+      </c>
+      <c r="U38">
+        <v>95</v>
+      </c>
+      <c r="V38">
+        <v>183</v>
+      </c>
+      <c r="W38">
+        <v>3753</v>
+      </c>
+      <c r="X38">
+        <v>417</v>
+      </c>
+      <c r="Y38">
+        <v>10</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26">
+      <c r="A39">
+        <v>0.7</v>
+      </c>
+      <c r="B39">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39">
+        <v>0.9501744680851065</v>
+      </c>
+      <c r="H39">
+        <v>0.9417035451217186</v>
+      </c>
+      <c r="I39">
+        <v>0.8925702410625336</v>
+      </c>
+      <c r="J39">
+        <v>0.9966877325581958</v>
+      </c>
+      <c r="K39">
+        <v>18.2</v>
+      </c>
+      <c r="L39">
+        <v>0.5</v>
+      </c>
+      <c r="M39">
+        <v>150.7</v>
+      </c>
+      <c r="N39">
+        <v>205.9</v>
+      </c>
+      <c r="O39">
+        <v>0.6572009291521486</v>
+      </c>
+      <c r="P39">
+        <v>0.5741199151725467</v>
+      </c>
+      <c r="Q39">
+        <v>0.581975867269985</v>
+      </c>
+      <c r="R39">
+        <v>0.5897692397116949</v>
+      </c>
+      <c r="S39">
+        <v>71</v>
+      </c>
+      <c r="T39">
+        <v>72</v>
+      </c>
+      <c r="U39">
+        <v>96</v>
+      </c>
+      <c r="V39">
+        <v>178</v>
+      </c>
+      <c r="W39">
+        <v>3753</v>
+      </c>
+      <c r="X39">
+        <v>417</v>
+      </c>
+      <c r="Y39">
+        <v>10</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26">
+      <c r="A40">
+        <v>0.7</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40">
+        <v>0.9619021276595745</v>
+      </c>
+      <c r="H40">
+        <v>0.9506759160193589</v>
+      </c>
+      <c r="I40">
+        <v>0.9892680533328045</v>
+      </c>
+      <c r="J40">
+        <v>0.9150914524428171</v>
+      </c>
+      <c r="K40">
+        <v>1.5</v>
+      </c>
+      <c r="L40">
+        <v>12.8</v>
+      </c>
+      <c r="M40">
+        <v>138.4</v>
+      </c>
+      <c r="N40">
+        <v>222.6</v>
+      </c>
+      <c r="O40">
+        <v>0.6543554006968642</v>
+      </c>
+      <c r="P40">
+        <v>0.4989387800397618</v>
+      </c>
+      <c r="Q40">
+        <v>0.6053649420754683</v>
+      </c>
+      <c r="R40">
+        <v>0.4547084056294582</v>
+      </c>
+      <c r="S40">
+        <v>52</v>
+      </c>
+      <c r="T40">
+        <v>92</v>
+      </c>
+      <c r="U40">
+        <v>76</v>
+      </c>
+      <c r="V40">
+        <v>197</v>
+      </c>
+      <c r="W40">
+        <v>3753</v>
+      </c>
+      <c r="X40">
+        <v>417</v>
+      </c>
+      <c r="Y40">
+        <v>10</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26">
+      <c r="A41">
+        <v>0.7</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41">
+        <v>0.9403127659574469</v>
+      </c>
+      <c r="H41">
+        <v>0.9306406979713817</v>
+      </c>
+      <c r="I41">
+        <v>0.8775601836552367</v>
+      </c>
+      <c r="J41">
+        <v>0.9907619491643571</v>
+      </c>
+      <c r="K41">
+        <v>21</v>
+      </c>
+      <c r="L41">
+        <v>1.4</v>
+      </c>
+      <c r="M41">
+        <v>149.8</v>
+      </c>
+      <c r="N41">
+        <v>203.1</v>
+      </c>
+      <c r="O41">
+        <v>0.645005807200929</v>
+      </c>
+      <c r="P41">
+        <v>0.5548898549233729</v>
+      </c>
+      <c r="Q41">
+        <v>0.555639655322318</v>
+      </c>
+      <c r="R41">
+        <v>0.5670804244774834</v>
+      </c>
+      <c r="S41">
+        <v>73</v>
+      </c>
+      <c r="T41">
+        <v>75</v>
+      </c>
+      <c r="U41">
+        <v>93</v>
+      </c>
+      <c r="V41">
+        <v>176</v>
+      </c>
+      <c r="W41">
+        <v>3753</v>
+      </c>
+      <c r="X41">
+        <v>417</v>
+      </c>
+      <c r="Y41">
+        <v>10</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26">
+      <c r="A42">
+        <v>0.7</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42">
+        <v>0.955768085106383</v>
+      </c>
+      <c r="H42">
+        <v>0.9480064848179628</v>
+      </c>
+      <c r="I42">
+        <v>0.9012270766939798</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>16.6</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>151.2</v>
+      </c>
+      <c r="N42">
+        <v>207.5</v>
+      </c>
+      <c r="O42">
+        <v>0.6860046457607432</v>
+      </c>
+      <c r="P42">
+        <v>0.5928711598712427</v>
+      </c>
+      <c r="Q42">
+        <v>0.6111204481792717</v>
+      </c>
+      <c r="R42">
+        <v>0.6027931488801055</v>
+      </c>
+      <c r="S42">
+        <v>63</v>
+      </c>
+      <c r="T42">
+        <v>68</v>
+      </c>
+      <c r="U42">
+        <v>100</v>
+      </c>
+      <c r="V42">
+        <v>186</v>
+      </c>
+      <c r="W42">
+        <v>3753</v>
+      </c>
+      <c r="X42">
+        <v>417</v>
+      </c>
+      <c r="Y42">
+        <v>10</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26">
+      <c r="A43">
+        <v>0.7</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43">
+        <v>0.9682921985815603</v>
+      </c>
+      <c r="H43">
+        <v>0.9594200776528229</v>
+      </c>
+      <c r="I43">
+        <v>0.9887179156952672</v>
+      </c>
+      <c r="J43">
+        <v>0.931864614525964</v>
+      </c>
+      <c r="K43">
         <v>1.6</v>
       </c>
-      <c r="M13">
-        <v>149.6</v>
-      </c>
-      <c r="N13">
-        <v>219.4</v>
-      </c>
-      <c r="O13">
-        <v>0.6473867595818814</v>
-      </c>
-      <c r="P13">
-        <v>0.5406489356920391</v>
-      </c>
-      <c r="Q13">
-        <v>0.5748298025503907</v>
-      </c>
-      <c r="R13">
-        <v>0.5233733230134159</v>
-      </c>
-      <c r="S13">
+      <c r="L43">
+        <v>10.3</v>
+      </c>
+      <c r="M43">
+        <v>140.9</v>
+      </c>
+      <c r="N43">
+        <v>222.5</v>
+      </c>
+      <c r="O43">
+        <v>0.6017421602787456</v>
+      </c>
+      <c r="P43">
+        <v>0.4464424225714548</v>
+      </c>
+      <c r="Q43">
+        <v>0.527518315018315</v>
+      </c>
+      <c r="R43">
+        <v>0.4095028113927023</v>
+      </c>
+      <c r="S43">
         <v>66</v>
       </c>
-      <c r="T13">
+      <c r="T43">
+        <v>100</v>
+      </c>
+      <c r="U43">
+        <v>68</v>
+      </c>
+      <c r="V43">
+        <v>183</v>
+      </c>
+      <c r="W43">
+        <v>3753</v>
+      </c>
+      <c r="X43">
+        <v>417</v>
+      </c>
+      <c r="Y43">
+        <v>10</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26">
+      <c r="A44">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0.9682914893617021</v>
+      </c>
+      <c r="H44">
+        <v>0.9622007181963437</v>
+      </c>
+      <c r="I44">
+        <v>0.9346113187491614</v>
+      </c>
+      <c r="J44">
+        <v>0.9920279007748327</v>
+      </c>
+      <c r="K44">
+        <v>10.7</v>
+      </c>
+      <c r="L44">
+        <v>1.2</v>
+      </c>
+      <c r="M44">
+        <v>150</v>
+      </c>
+      <c r="N44">
+        <v>213.4</v>
+      </c>
+      <c r="O44">
+        <v>0.6310104529616724</v>
+      </c>
+      <c r="P44">
+        <v>0.5463907497746459</v>
+      </c>
+      <c r="Q44">
+        <v>0.5466131580837462</v>
+      </c>
+      <c r="R44">
+        <v>0.5553459631520272</v>
+      </c>
+      <c r="S44">
+        <v>80</v>
+      </c>
+      <c r="T44">
+        <v>74</v>
+      </c>
+      <c r="U44">
+        <v>94</v>
+      </c>
+      <c r="V44">
+        <v>169</v>
+      </c>
+      <c r="W44">
+        <v>3753</v>
+      </c>
+      <c r="X44">
+        <v>417</v>
+      </c>
+      <c r="Y44">
+        <v>10</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26">
+      <c r="A45">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B45">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0.9738872340425532</v>
+      </c>
+      <c r="H45">
+        <v>0.9683190298525371</v>
+      </c>
+      <c r="I45">
+        <v>0.9471224546806301</v>
+      </c>
+      <c r="J45">
+        <v>0.9906500565828298</v>
+      </c>
+      <c r="K45">
+        <v>8.4</v>
+      </c>
+      <c r="L45">
+        <v>1.4</v>
+      </c>
+      <c r="M45">
+        <v>149.8</v>
+      </c>
+      <c r="N45">
+        <v>215.7</v>
+      </c>
+      <c r="O45">
+        <v>0.6305458768873403</v>
+      </c>
+      <c r="P45">
+        <v>0.5273072284023048</v>
+      </c>
+      <c r="Q45">
+        <v>0.5390428418330895</v>
+      </c>
+      <c r="R45">
+        <v>0.5252059125085441</v>
+      </c>
+      <c r="S45">
+        <v>75</v>
+      </c>
+      <c r="T45">
+        <v>79</v>
+      </c>
+      <c r="U45">
+        <v>89</v>
+      </c>
+      <c r="V45">
+        <v>174</v>
+      </c>
+      <c r="W45">
+        <v>3753</v>
+      </c>
+      <c r="X45">
+        <v>417</v>
+      </c>
+      <c r="Y45">
+        <v>10</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26">
+      <c r="A46">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0.9560368794326243</v>
+      </c>
+      <c r="H46">
+        <v>0.9448112110715907</v>
+      </c>
+      <c r="I46">
+        <v>0.9567696826724077</v>
+      </c>
+      <c r="J46">
+        <v>0.9332155228253649</v>
+      </c>
+      <c r="K46">
+        <v>6.4</v>
+      </c>
+      <c r="L46">
+        <v>10.1</v>
+      </c>
+      <c r="M46">
+        <v>141.1</v>
+      </c>
+      <c r="N46">
+        <v>217.7</v>
+      </c>
+      <c r="O46">
+        <v>0.6855981416957025</v>
+      </c>
+      <c r="P46">
+        <v>0.5764509060638092</v>
+      </c>
+      <c r="Q46">
+        <v>0.6226548889706784</v>
+      </c>
+      <c r="R46">
+        <v>0.5548906837169053</v>
+      </c>
+      <c r="S46">
+        <v>56</v>
+      </c>
+      <c r="T46">
+        <v>75</v>
+      </c>
+      <c r="U46">
+        <v>93</v>
+      </c>
+      <c r="V46">
+        <v>193</v>
+      </c>
+      <c r="W46">
+        <v>3753</v>
+      </c>
+      <c r="X46">
+        <v>417</v>
+      </c>
+      <c r="Y46">
+        <v>10</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26">
+      <c r="A47">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47">
+        <v>0.9712255319148936</v>
+      </c>
+      <c r="H47">
+        <v>0.9654616694136117</v>
+      </c>
+      <c r="I47">
+        <v>0.9385985119447605</v>
+      </c>
+      <c r="J47">
+        <v>0.9940688399012239</v>
+      </c>
+      <c r="K47">
+        <v>9.9</v>
+      </c>
+      <c r="L47">
+        <v>0.9</v>
+      </c>
+      <c r="M47">
+        <v>150.3</v>
+      </c>
+      <c r="N47">
+        <v>214.2</v>
+      </c>
+      <c r="O47">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="P47">
+        <v>0.5481379961970161</v>
+      </c>
+      <c r="Q47">
+        <v>0.5711617485275007</v>
+      </c>
+      <c r="R47">
+        <v>0.5383004078824511</v>
+      </c>
+      <c r="S47">
+        <v>70</v>
+      </c>
+      <c r="T47">
+        <v>76</v>
+      </c>
+      <c r="U47">
+        <v>92</v>
+      </c>
+      <c r="V47">
+        <v>179</v>
+      </c>
+      <c r="W47">
+        <v>3753</v>
+      </c>
+      <c r="X47">
+        <v>417</v>
+      </c>
+      <c r="Y47">
+        <v>10</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26">
+      <c r="A48">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B48">
+        <v>30</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48">
+        <v>0.9912085106382978</v>
+      </c>
+      <c r="H48">
+        <v>0.9890499346141303</v>
+      </c>
+      <c r="I48">
+        <v>0.9874580114119386</v>
+      </c>
+      <c r="J48">
+        <v>0.9906703476883884</v>
+      </c>
+      <c r="K48">
+        <v>1.9</v>
+      </c>
+      <c r="L48">
+        <v>1.4</v>
+      </c>
+      <c r="M48">
+        <v>149.8</v>
+      </c>
+      <c r="N48">
+        <v>222.2</v>
+      </c>
+      <c r="O48">
+        <v>0.6304297328687571</v>
+      </c>
+      <c r="P48">
+        <v>0.5233334253233244</v>
+      </c>
+      <c r="Q48">
+        <v>0.5423150825782406</v>
+      </c>
+      <c r="R48">
+        <v>0.5127808302808303</v>
+      </c>
+      <c r="S48">
+        <v>72</v>
+      </c>
+      <c r="T48">
+        <v>82</v>
+      </c>
+      <c r="U48">
+        <v>86</v>
+      </c>
+      <c r="V48">
+        <v>177</v>
+      </c>
+      <c r="W48">
+        <v>3753</v>
+      </c>
+      <c r="X48">
+        <v>417</v>
+      </c>
+      <c r="Y48">
+        <v>10</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26">
+      <c r="A49">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B49">
+        <v>30</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49">
+        <v>0.9810815602836879</v>
+      </c>
+      <c r="H49">
+        <v>0.9767974696422158</v>
+      </c>
+      <c r="I49">
+        <v>0.9658970348121821</v>
+      </c>
+      <c r="J49">
+        <v>0.9880504925653003</v>
+      </c>
+      <c r="K49">
+        <v>5.3</v>
+      </c>
+      <c r="L49">
+        <v>1.8</v>
+      </c>
+      <c r="M49">
+        <v>149.4</v>
+      </c>
+      <c r="N49">
+        <v>218.8</v>
+      </c>
+      <c r="O49">
+        <v>0.6641114982578397</v>
+      </c>
+      <c r="P49">
+        <v>0.5761714138184727</v>
+      </c>
+      <c r="Q49">
+        <v>0.5934090586168592</v>
+      </c>
+      <c r="R49">
+        <v>0.5758851348170233</v>
+      </c>
+      <c r="S49">
+        <v>69</v>
+      </c>
+      <c r="T49">
+        <v>71</v>
+      </c>
+      <c r="U49">
+        <v>97</v>
+      </c>
+      <c r="V49">
+        <v>180</v>
+      </c>
+      <c r="W49">
+        <v>3753</v>
+      </c>
+      <c r="X49">
+        <v>417</v>
+      </c>
+      <c r="Y49">
+        <v>10</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26">
+      <c r="A50">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B50">
+        <v>30</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50">
+        <v>0.9592326241134753</v>
+      </c>
+      <c r="H50">
+        <v>0.9515898390352167</v>
+      </c>
+      <c r="I50">
+        <v>0.9132787302563095</v>
+      </c>
+      <c r="J50">
+        <v>0.9933526883201113</v>
+      </c>
+      <c r="K50">
+        <v>14.3</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>150.2</v>
+      </c>
+      <c r="N50">
+        <v>209.8</v>
+      </c>
+      <c r="O50">
+        <v>0.6858304297328687</v>
+      </c>
+      <c r="P50">
+        <v>0.6151695644503994</v>
+      </c>
+      <c r="Q50">
+        <v>0.6067043816463321</v>
+      </c>
+      <c r="R50">
+        <v>0.6495798319327731</v>
+      </c>
+      <c r="S50">
+        <v>72</v>
+      </c>
+      <c r="T50">
+        <v>59</v>
+      </c>
+      <c r="U50">
+        <v>109</v>
+      </c>
+      <c r="V50">
+        <v>177</v>
+      </c>
+      <c r="W50">
+        <v>3753</v>
+      </c>
+      <c r="X50">
+        <v>417</v>
+      </c>
+      <c r="Y50">
+        <v>10</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26">
+      <c r="A51">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B51">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51">
+        <v>0.9834794326241134</v>
+      </c>
+      <c r="H51">
+        <v>0.9796655126358749</v>
+      </c>
+      <c r="I51">
+        <v>0.9741992917932583</v>
+      </c>
+      <c r="J51">
+        <v>0.985375222148078</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <v>2.2</v>
+      </c>
+      <c r="M51">
+        <v>149</v>
+      </c>
+      <c r="N51">
+        <v>220.1</v>
+      </c>
+      <c r="O51">
+        <v>0.6595818815331009</v>
+      </c>
+      <c r="P51">
+        <v>0.5585060827850202</v>
+      </c>
+      <c r="Q51">
+        <v>0.6028940422322775</v>
+      </c>
+      <c r="R51">
+        <v>0.5587741579885543</v>
+      </c>
+      <c r="S51">
+        <v>64</v>
+      </c>
+      <c r="T51">
+        <v>78</v>
+      </c>
+      <c r="U51">
+        <v>90</v>
+      </c>
+      <c r="V51">
+        <v>185</v>
+      </c>
+      <c r="W51">
+        <v>3753</v>
+      </c>
+      <c r="X51">
+        <v>417</v>
+      </c>
+      <c r="Y51">
+        <v>10</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26">
+      <c r="A52">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B52">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52">
+        <v>0.97255390070922</v>
+      </c>
+      <c r="H52">
+        <v>0.9665659542016403</v>
+      </c>
+      <c r="I52">
+        <v>0.9485464943475478</v>
+      </c>
+      <c r="J52">
+        <v>0.9853621139208008</v>
+      </c>
+      <c r="K52">
+        <v>8.1</v>
+      </c>
+      <c r="L52">
+        <v>2.2</v>
+      </c>
+      <c r="M52">
+        <v>149</v>
+      </c>
+      <c r="N52">
+        <v>216</v>
+      </c>
+      <c r="O52">
+        <v>0.6592915214866433</v>
+      </c>
+      <c r="P52">
+        <v>0.5714425827926422</v>
+      </c>
+      <c r="Q52">
+        <v>0.5839930709125756</v>
+      </c>
+      <c r="R52">
+        <v>0.5722197603737851</v>
+      </c>
+      <c r="S52">
+        <v>69</v>
+      </c>
+      <c r="T52">
+        <v>73</v>
+      </c>
+      <c r="U52">
+        <v>95</v>
+      </c>
+      <c r="V52">
+        <v>180</v>
+      </c>
+      <c r="W52">
+        <v>3753</v>
+      </c>
+      <c r="X52">
+        <v>417</v>
+      </c>
+      <c r="Y52">
+        <v>10</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26">
+      <c r="A53">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B53">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53">
+        <v>0.9693581560283689</v>
+      </c>
+      <c r="H53">
+        <v>0.9633035201067683</v>
+      </c>
+      <c r="I53">
+        <v>0.9321578450876468</v>
+      </c>
+      <c r="J53">
+        <v>0.9966796200383052</v>
+      </c>
+      <c r="K53">
+        <v>11</v>
+      </c>
+      <c r="L53">
+        <v>0.5</v>
+      </c>
+      <c r="M53">
+        <v>150.7</v>
+      </c>
+      <c r="N53">
+        <v>213.1</v>
+      </c>
+      <c r="O53">
+        <v>0.6499419279907084</v>
+      </c>
+      <c r="P53">
+        <v>0.5571809439859321</v>
+      </c>
+      <c r="Q53">
+        <v>0.5854586203270413</v>
+      </c>
+      <c r="R53">
+        <v>0.5484693930940061</v>
+      </c>
+      <c r="S53">
+        <v>69</v>
+      </c>
+      <c r="T53">
+        <v>77</v>
+      </c>
+      <c r="U53">
+        <v>91</v>
+      </c>
+      <c r="V53">
+        <v>180</v>
+      </c>
+      <c r="W53">
+        <v>3753</v>
+      </c>
+      <c r="X53">
+        <v>417</v>
+      </c>
+      <c r="Y53">
+        <v>10</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26">
+      <c r="A54">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B54">
+        <v>30</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54">
+        <v>0.9730851063829787</v>
+      </c>
+      <c r="H54">
+        <v>0.9677366316270988</v>
+      </c>
+      <c r="I54">
+        <v>0.9417861265171489</v>
+      </c>
+      <c r="J54">
+        <v>0.9953583657406349</v>
+      </c>
+      <c r="K54">
+        <v>9.4</v>
+      </c>
+      <c r="L54">
+        <v>0.7</v>
+      </c>
+      <c r="M54">
+        <v>150.5</v>
+      </c>
+      <c r="N54">
+        <v>214.7</v>
+      </c>
+      <c r="O54">
+        <v>0.6573751451800232</v>
+      </c>
+      <c r="P54">
+        <v>0.5816687595382</v>
+      </c>
+      <c r="Q54">
+        <v>0.5797510705743307</v>
+      </c>
+      <c r="R54">
+        <v>0.6153667823404666</v>
+      </c>
+      <c r="S54">
+        <v>77</v>
+      </c>
+      <c r="T54">
+        <v>66</v>
+      </c>
+      <c r="U54">
+        <v>102</v>
+      </c>
+      <c r="V54">
+        <v>172</v>
+      </c>
+      <c r="W54">
+        <v>3753</v>
+      </c>
+      <c r="X54">
+        <v>417</v>
+      </c>
+      <c r="Y54">
+        <v>10</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26">
+      <c r="A55">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="B55">
+        <v>30</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55">
+        <v>0.9912042553191489</v>
+      </c>
+      <c r="H55">
+        <v>0.9892384520194302</v>
+      </c>
+      <c r="I55">
+        <v>0.983294820251459</v>
+      </c>
+      <c r="J55">
+        <v>0.9953453509167793</v>
+      </c>
+      <c r="K55">
+        <v>2.6</v>
+      </c>
+      <c r="L55">
+        <v>0.7</v>
+      </c>
+      <c r="M55">
+        <v>150.5</v>
+      </c>
+      <c r="N55">
+        <v>221.5</v>
+      </c>
+      <c r="O55">
+        <v>0.6573170731707316</v>
+      </c>
+      <c r="P55">
+        <v>0.5553030968682346</v>
+      </c>
+      <c r="Q55">
+        <v>0.5817924902754624</v>
+      </c>
+      <c r="R55">
+        <v>0.5574603174603173</v>
+      </c>
+      <c r="S55">
+        <v>66</v>
+      </c>
+      <c r="T55">
+        <v>77</v>
+      </c>
+      <c r="U55">
+        <v>91</v>
+      </c>
+      <c r="V55">
+        <v>183</v>
+      </c>
+      <c r="W55">
+        <v>3753</v>
+      </c>
+      <c r="X55">
+        <v>417</v>
+      </c>
+      <c r="Y55">
+        <v>10</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26">
+      <c r="A56">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="B56">
+        <v>30</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0.9744191489361702</v>
+      </c>
+      <c r="H56">
+        <v>0.969186229549322</v>
+      </c>
+      <c r="I56">
+        <v>0.9445288146616901</v>
+      </c>
+      <c r="J56">
+        <v>0.9953376309902273</v>
+      </c>
+      <c r="K56">
+        <v>8.9</v>
+      </c>
+      <c r="L56">
+        <v>0.7</v>
+      </c>
+      <c r="M56">
+        <v>150.5</v>
+      </c>
+      <c r="N56">
+        <v>215.2</v>
+      </c>
+      <c r="O56">
+        <v>0.6523809523809523</v>
+      </c>
+      <c r="P56">
+        <v>0.5604772182400103</v>
+      </c>
+      <c r="Q56">
+        <v>0.5682594070016671</v>
+      </c>
+      <c r="R56">
+        <v>0.5553008322087269</v>
+      </c>
+      <c r="S56">
+        <v>71</v>
+      </c>
+      <c r="T56">
+        <v>74</v>
+      </c>
+      <c r="U56">
+        <v>94</v>
+      </c>
+      <c r="V56">
+        <v>178</v>
+      </c>
+      <c r="W56">
+        <v>3753</v>
+      </c>
+      <c r="X56">
+        <v>417</v>
+      </c>
+      <c r="Y56">
+        <v>10</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26">
+      <c r="A57">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="B57">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0.9834801418439717</v>
+      </c>
+      <c r="H57">
+        <v>0.979877807657289</v>
+      </c>
+      <c r="I57">
+        <v>0.9650076416701342</v>
+      </c>
+      <c r="J57">
+        <v>0.9953408195722794</v>
+      </c>
+      <c r="K57">
+        <v>5.5</v>
+      </c>
+      <c r="L57">
+        <v>0.7</v>
+      </c>
+      <c r="M57">
+        <v>150.5</v>
+      </c>
+      <c r="N57">
+        <v>218.6</v>
+      </c>
+      <c r="O57">
+        <v>0.6397793263646923</v>
+      </c>
+      <c r="P57">
+        <v>0.547506394592578</v>
+      </c>
+      <c r="Q57">
+        <v>0.5586088506548865</v>
+      </c>
+      <c r="R57">
+        <v>0.5516062261611798</v>
+      </c>
+      <c r="S57">
+        <v>72</v>
+      </c>
+      <c r="T57">
+        <v>78</v>
+      </c>
+      <c r="U57">
+        <v>90</v>
+      </c>
+      <c r="V57">
+        <v>177</v>
+      </c>
+      <c r="W57">
+        <v>3753</v>
+      </c>
+      <c r="X57">
+        <v>417</v>
+      </c>
+      <c r="Y57">
+        <v>10</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26">
+      <c r="A58">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="B58">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0.982413475177305</v>
+      </c>
+      <c r="H58">
+        <v>0.9787520870199252</v>
+      </c>
+      <c r="I58">
+        <v>0.9591111940413256</v>
+      </c>
+      <c r="J58">
+        <v>0.9993464052287582</v>
+      </c>
+      <c r="K58">
+        <v>6.5</v>
+      </c>
+      <c r="L58">
+        <v>0.1</v>
+      </c>
+      <c r="M58">
+        <v>151.1</v>
+      </c>
+      <c r="N58">
+        <v>217.6</v>
+      </c>
+      <c r="O58">
+        <v>0.6452961672473867</v>
+      </c>
+      <c r="P58">
+        <v>0.5342372462596654</v>
+      </c>
+      <c r="Q58">
+        <v>0.5616447368421053</v>
+      </c>
+      <c r="R58">
+        <v>0.5205320711280464</v>
+      </c>
+      <c r="S58">
+        <v>67</v>
+      </c>
+      <c r="T58">
         <v>81</v>
       </c>
-      <c r="U13">
+      <c r="U58">
         <v>87</v>
       </c>
-      <c r="V13">
-        <v>183</v>
-      </c>
-      <c r="W13">
-        <v>3753</v>
-      </c>
-      <c r="X13">
-        <v>417</v>
-      </c>
-      <c r="Y13">
-        <v>10</v>
-      </c>
-      <c r="Z13" t="s">
+      <c r="V58">
+        <v>182</v>
+      </c>
+      <c r="W58">
+        <v>3753</v>
+      </c>
+      <c r="X58">
+        <v>417</v>
+      </c>
+      <c r="Y58">
+        <v>10</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26">
+      <c r="A59">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" t="s">
         <v>28</v>
+      </c>
+      <c r="G59">
+        <v>0.989609929078014</v>
+      </c>
+      <c r="H59">
+        <v>0.9872017107120052</v>
+      </c>
+      <c r="I59">
+        <v>0.9844435162958955</v>
+      </c>
+      <c r="J59">
+        <v>0.9900688385214215</v>
+      </c>
+      <c r="K59">
+        <v>2.4</v>
+      </c>
+      <c r="L59">
+        <v>1.5</v>
+      </c>
+      <c r="M59">
+        <v>149.7</v>
+      </c>
+      <c r="N59">
+        <v>221.7</v>
+      </c>
+      <c r="O59">
+        <v>0.6429152148664342</v>
+      </c>
+      <c r="P59">
+        <v>0.5338121370008848</v>
+      </c>
+      <c r="Q59">
+        <v>0.5645396708554603</v>
+      </c>
+      <c r="R59">
+        <v>0.5112271062271062</v>
+      </c>
+      <c r="S59">
+        <v>67</v>
+      </c>
+      <c r="T59">
+        <v>82</v>
+      </c>
+      <c r="U59">
+        <v>86</v>
+      </c>
+      <c r="V59">
+        <v>182</v>
+      </c>
+      <c r="W59">
+        <v>3753</v>
+      </c>
+      <c r="X59">
+        <v>417</v>
+      </c>
+      <c r="Y59">
+        <v>10</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>